<commit_message>
31.12.20 all repositories finished
</commit_message>
<xml_diff>
--- a/Spectral_data/Occupancies_out.xlsx
+++ b/Spectral_data/Occupancies_out.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="12">
   <si>
-    <t>16/12/2020 18:58</t>
+    <t>30/12/2020 13:29</t>
   </si>
   <si>
     <t>fragmentation:</t>
@@ -256,43 +256,40 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.6529328164199616</c:v>
+                  <c:v>0.6041451629601375</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.8112504716822778</c:v>
+                  <c:v>0.6728636349042659</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.8307858240249646</c:v>
+                  <c:v>0.6625332575470484</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.7720389018061461</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.6916614430054613</c:v>
+                  <c:v>0.5883708159472228</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.6280941588521683</c:v>
+                  <c:v>0.6728692038737724</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.738166035780348</c:v>
+                  <c:v>0.8018253063751378</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.8337828134846464</c:v>
+                  <c:v>0.8242511977940842</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1</c:v>
+                  <c:v>0.9223260847425075</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1</c:v>
+                  <c:v>0.9377312342782025</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1</c:v>
+                  <c:v>0.9695901174831573</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1</c:v>
+                  <c:v>0.940240303617473</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>1</c:v>
@@ -456,38 +453,35 @@
                 <c:pt idx="5">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.2718965394974235</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.14124508163094</c:v>
+                  <c:v>0.2168778351840947</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.1252412080589887</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.09586643633666368</c:v>
+                  <c:v>0.2614169773890365</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.1584709962663967</c:v>
+                  <c:v>0.2242293832902997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.2472455243504849</c:v>
+                  <c:v>0.175136125606864</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.140279755416884</c:v>
+                  <c:v>0.1291571788194893</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.1594902835556192</c:v>
+                  <c:v>0.05298865377612615</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>0.05198800502692182</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>0.03734325373602206</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0</c:v>
@@ -1027,7 +1021,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>0.4713669127906773</v>
+        <v>0.4386471720076599</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1035,7 +1029,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>0.528633087209323</v>
+        <v>0.5613528279923402</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1167,10 +1161,7 @@
         <v>7</v>
       </c>
       <c r="C15" s="1">
-        <v>0.6529328164199616</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0.2718965394974235</v>
+        <v>0.6041451629601375</v>
       </c>
       <c r="E15">
         <v>20</v>
@@ -1184,10 +1175,10 @@
         <v>8</v>
       </c>
       <c r="C16" s="1">
-        <v>0.8112504716822778</v>
+        <v>0.6728636349042659</v>
       </c>
       <c r="D16" s="1">
-        <v>0.14124508163094</v>
+        <v>0.2168778351840947</v>
       </c>
       <c r="E16">
         <v>19</v>
@@ -1201,10 +1192,10 @@
         <v>9</v>
       </c>
       <c r="C17" s="1">
-        <v>0.8307858240249646</v>
+        <v>0.6625332575470484</v>
       </c>
       <c r="D17" s="1">
-        <v>0</v>
+        <v>0.1252412080589887</v>
       </c>
       <c r="E17">
         <v>18</v>
@@ -1218,10 +1209,10 @@
         <v>10</v>
       </c>
       <c r="C18" s="1">
-        <v>0.7720389018061461</v>
+        <v>0.5883708159472228</v>
       </c>
       <c r="D18" s="1">
-        <v>0.09586643633666368</v>
+        <v>0.2614169773890365</v>
       </c>
       <c r="E18">
         <v>17</v>
@@ -1234,11 +1225,8 @@
       <c r="B19">
         <v>11</v>
       </c>
-      <c r="C19" s="1">
-        <v>0.6916614430054613</v>
-      </c>
       <c r="D19" s="1">
-        <v>0.1584709962663967</v>
+        <v>0.2242293832902997</v>
       </c>
       <c r="E19">
         <v>16</v>
@@ -1252,10 +1240,10 @@
         <v>12</v>
       </c>
       <c r="C20" s="1">
-        <v>0.6280941588521683</v>
+        <v>0.6728692038737724</v>
       </c>
       <c r="D20" s="1">
-        <v>0.2472455243504849</v>
+        <v>0.175136125606864</v>
       </c>
       <c r="E20">
         <v>15</v>
@@ -1269,10 +1257,10 @@
         <v>13</v>
       </c>
       <c r="C21" s="1">
-        <v>0.738166035780348</v>
+        <v>0.8018253063751378</v>
       </c>
       <c r="D21" s="1">
-        <v>0.140279755416884</v>
+        <v>0.1291571788194893</v>
       </c>
       <c r="E21">
         <v>14</v>
@@ -1286,10 +1274,10 @@
         <v>14</v>
       </c>
       <c r="C22" s="1">
-        <v>0.8337828134846464</v>
+        <v>0.8242511977940842</v>
       </c>
       <c r="D22" s="1">
-        <v>0.1594902835556192</v>
+        <v>0.05298865377612615</v>
       </c>
       <c r="E22">
         <v>13</v>
@@ -1303,7 +1291,7 @@
         <v>15</v>
       </c>
       <c r="C23" s="1">
-        <v>1</v>
+        <v>0.9223260847425075</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
@@ -1320,10 +1308,10 @@
         <v>16</v>
       </c>
       <c r="C24" s="1">
-        <v>1</v>
+        <v>0.9377312342782025</v>
       </c>
       <c r="D24" s="1">
-        <v>0</v>
+        <v>0.05198800502692182</v>
       </c>
       <c r="E24">
         <v>11</v>
@@ -1340,7 +1328,7 @@
         <v>1</v>
       </c>
       <c r="D25" s="1">
-        <v>0</v>
+        <v>0.03734325373602206</v>
       </c>
       <c r="E25">
         <v>10</v>
@@ -1354,7 +1342,7 @@
         <v>18</v>
       </c>
       <c r="C26" s="1">
-        <v>1</v>
+        <v>0.9695901174831573</v>
       </c>
       <c r="D26" s="1">
         <v>0</v>
@@ -1371,7 +1359,7 @@
         <v>19</v>
       </c>
       <c r="C27" s="1">
-        <v>1</v>
+        <v>0.940240303617473</v>
       </c>
       <c r="D27" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
09.01.21 updated version of FragmentsAndModifs.py and corresponding service
</commit_message>
<xml_diff>
--- a/Spectral_data/Occupancies_out.xlsx
+++ b/Spectral_data/Occupancies_out.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="12">
   <si>
-    <t>30/12/2020 13:29</t>
+    <t>05/01/2021 07:19</t>
   </si>
   <si>
     <t>fragmentation:</t>
@@ -240,6 +240,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
@@ -256,40 +259,40 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.6041451629601375</c:v>
+                  <c:v>0.4897753206044688</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.6728636349042659</c:v>
+                  <c:v>0.7251818265247796</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.6625332575470484</c:v>
+                  <c:v>0.5930301556535866</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.5883708159472228</c:v>
+                  <c:v>0.5957613279533805</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.6728692038737724</c:v>
+                  <c:v>0.7099376897136177</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.8018253063751378</c:v>
+                  <c:v>0.7725343881445893</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.8242511977940842</c:v>
+                  <c:v>0.7534560635001963</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.9223260847425075</c:v>
+                  <c:v>0.9411399939792753</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.9377312342782025</c:v>
+                  <c:v>0.8859485205328446</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1</c:v>
+                  <c:v>0.9378870897892354</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.9695901174831573</c:v>
+                  <c:v>0.9559561959853398</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.940240303617473</c:v>
+                  <c:v>0.9589717608419112</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>1</c:v>
@@ -451,37 +454,37 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0.8635498221650165</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.2168778351840947</c:v>
+                  <c:v>0.2402247305710664</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.1252412080589887</c:v>
+                  <c:v>0.1916542514218098</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.2614169773890365</c:v>
+                  <c:v>0.2823111139439658</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.2242293832902997</c:v>
+                  <c:v>0.1975815868176595</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.175136125606864</c:v>
+                  <c:v>0.113648553805877</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.1291571788194893</c:v>
+                  <c:v>0.1971928126262711</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.05298865377612615</c:v>
+                  <c:v>0.101893287078088</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>0.03457147852972665</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.06280325380231767</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.05198800502692182</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.03734325373602206</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0</c:v>
@@ -1021,7 +1024,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>0.4386471720076599</v>
+        <v>0.4251975800471628</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1029,7 +1032,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>0.5613528279923402</v>
+        <v>0.574802419952838</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1061,6 +1064,9 @@
       <c r="B9">
         <v>1</v>
       </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
       <c r="D9" s="1">
         <v>1</v>
       </c>
@@ -1147,7 +1153,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="1">
-        <v>1</v>
+        <v>0.8635498221650165</v>
       </c>
       <c r="E14">
         <v>21</v>
@@ -1161,7 +1167,7 @@
         <v>7</v>
       </c>
       <c r="C15" s="1">
-        <v>0.6041451629601375</v>
+        <v>0.4897753206044688</v>
       </c>
       <c r="E15">
         <v>20</v>
@@ -1175,10 +1181,10 @@
         <v>8</v>
       </c>
       <c r="C16" s="1">
-        <v>0.6728636349042659</v>
+        <v>0.7251818265247796</v>
       </c>
       <c r="D16" s="1">
-        <v>0.2168778351840947</v>
+        <v>0.2402247305710664</v>
       </c>
       <c r="E16">
         <v>19</v>
@@ -1192,10 +1198,10 @@
         <v>9</v>
       </c>
       <c r="C17" s="1">
-        <v>0.6625332575470484</v>
+        <v>0.5930301556535866</v>
       </c>
       <c r="D17" s="1">
-        <v>0.1252412080589887</v>
+        <v>0.1916542514218098</v>
       </c>
       <c r="E17">
         <v>18</v>
@@ -1209,10 +1215,10 @@
         <v>10</v>
       </c>
       <c r="C18" s="1">
-        <v>0.5883708159472228</v>
+        <v>0.5957613279533805</v>
       </c>
       <c r="D18" s="1">
-        <v>0.2614169773890365</v>
+        <v>0.2823111139439658</v>
       </c>
       <c r="E18">
         <v>17</v>
@@ -1226,7 +1232,7 @@
         <v>11</v>
       </c>
       <c r="D19" s="1">
-        <v>0.2242293832902997</v>
+        <v>0.1975815868176595</v>
       </c>
       <c r="E19">
         <v>16</v>
@@ -1240,10 +1246,10 @@
         <v>12</v>
       </c>
       <c r="C20" s="1">
-        <v>0.6728692038737724</v>
+        <v>0.7099376897136177</v>
       </c>
       <c r="D20" s="1">
-        <v>0.175136125606864</v>
+        <v>0.113648553805877</v>
       </c>
       <c r="E20">
         <v>15</v>
@@ -1257,10 +1263,10 @@
         <v>13</v>
       </c>
       <c r="C21" s="1">
-        <v>0.8018253063751378</v>
+        <v>0.7725343881445893</v>
       </c>
       <c r="D21" s="1">
-        <v>0.1291571788194893</v>
+        <v>0.1971928126262711</v>
       </c>
       <c r="E21">
         <v>14</v>
@@ -1274,10 +1280,10 @@
         <v>14</v>
       </c>
       <c r="C22" s="1">
-        <v>0.8242511977940842</v>
+        <v>0.7534560635001963</v>
       </c>
       <c r="D22" s="1">
-        <v>0.05298865377612615</v>
+        <v>0.101893287078088</v>
       </c>
       <c r="E22">
         <v>13</v>
@@ -1291,10 +1297,10 @@
         <v>15</v>
       </c>
       <c r="C23" s="1">
-        <v>0.9223260847425075</v>
+        <v>0.9411399939792753</v>
       </c>
       <c r="D23" s="1">
-        <v>0</v>
+        <v>0.03457147852972665</v>
       </c>
       <c r="E23">
         <v>12</v>
@@ -1308,10 +1314,10 @@
         <v>16</v>
       </c>
       <c r="C24" s="1">
-        <v>0.9377312342782025</v>
+        <v>0.8859485205328446</v>
       </c>
       <c r="D24" s="1">
-        <v>0.05198800502692182</v>
+        <v>0.06280325380231767</v>
       </c>
       <c r="E24">
         <v>11</v>
@@ -1325,10 +1331,10 @@
         <v>17</v>
       </c>
       <c r="C25" s="1">
-        <v>1</v>
+        <v>0.9378870897892354</v>
       </c>
       <c r="D25" s="1">
-        <v>0.03734325373602206</v>
+        <v>0</v>
       </c>
       <c r="E25">
         <v>10</v>
@@ -1342,7 +1348,7 @@
         <v>18</v>
       </c>
       <c r="C26" s="1">
-        <v>0.9695901174831573</v>
+        <v>0.9559561959853398</v>
       </c>
       <c r="D26" s="1">
         <v>0</v>
@@ -1359,7 +1365,7 @@
         <v>19</v>
       </c>
       <c r="C27" s="1">
-        <v>0.940240303617473</v>
+        <v>0.9589717608419112</v>
       </c>
       <c r="D27" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
14.01.21 Filled all databases excluding modifications and intact modifications, debugging
</commit_message>
<xml_diff>
--- a/Spectral_data/Occupancies_out.xlsx
+++ b/Spectral_data/Occupancies_out.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="12">
   <si>
-    <t>05/01/2021 07:19</t>
+    <t>11/01/2021 17:56</t>
   </si>
   <si>
     <t>fragmentation:</t>
@@ -240,9 +240,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
@@ -259,40 +256,43 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.4897753206044688</c:v>
+                  <c:v>0.2948192554489688</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.7251818265247796</c:v>
+                  <c:v>0.3089824189933628</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.5930301556535866</c:v>
+                  <c:v>0.3091405136994379</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.5957613279533805</c:v>
+                  <c:v>0.3166188715203264</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.7099376897136177</c:v>
+                  <c:v>0.3676918970110236</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.7725343881445893</c:v>
+                  <c:v>0.5694399995102261</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.7534560635001963</c:v>
+                  <c:v>0.6968909473354162</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.9411399939792753</c:v>
+                  <c:v>0.7322849197478155</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.8859485205328446</c:v>
+                  <c:v>0.6805195656183084</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.9378870897892354</c:v>
+                  <c:v>0.871710627973019</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.9559561959853398</c:v>
+                  <c:v>0.9542488324553626</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.9589717608419112</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>1</c:v>
@@ -454,43 +454,43 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.8635498221650165</c:v>
+                  <c:v>0.9426793405802766</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.2402247305710664</c:v>
+                  <c:v>0.5904833814888236</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.1916542514218098</c:v>
+                  <c:v>0.5877238379963322</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.2823111139439658</c:v>
+                  <c:v>0.6950272937821849</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.1975815868176595</c:v>
+                  <c:v>0.4799780978171799</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.113648553805877</c:v>
+                  <c:v>0.4964041833034137</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.1971928126262711</c:v>
+                  <c:v>0.4511452428471781</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.101893287078088</c:v>
+                  <c:v>0.1808410096349255</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.03457147852972665</c:v>
+                  <c:v>0.1557090277338459</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.06280325380231767</c:v>
+                  <c:v>0.2110274212379415</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>0.2286928381609282</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>0.044303539091117</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>0.0865902006984151</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
@@ -1024,7 +1024,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>0.4251975800471628</v>
+        <v>0.4586934551182387</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1032,7 +1032,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>0.574802419952838</v>
+        <v>0.5413065448817613</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1064,9 +1064,6 @@
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9" s="1">
-        <v>0</v>
-      </c>
       <c r="D9" s="1">
         <v>1</v>
       </c>
@@ -1153,7 +1150,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="1">
-        <v>0.8635498221650165</v>
+        <v>0.9426793405802766</v>
       </c>
       <c r="E14">
         <v>21</v>
@@ -1167,7 +1164,7 @@
         <v>7</v>
       </c>
       <c r="C15" s="1">
-        <v>0.4897753206044688</v>
+        <v>0.2948192554489688</v>
       </c>
       <c r="E15">
         <v>20</v>
@@ -1181,10 +1178,10 @@
         <v>8</v>
       </c>
       <c r="C16" s="1">
-        <v>0.7251818265247796</v>
+        <v>0.3089824189933628</v>
       </c>
       <c r="D16" s="1">
-        <v>0.2402247305710664</v>
+        <v>0.5904833814888236</v>
       </c>
       <c r="E16">
         <v>19</v>
@@ -1198,10 +1195,10 @@
         <v>9</v>
       </c>
       <c r="C17" s="1">
-        <v>0.5930301556535866</v>
+        <v>0.3091405136994379</v>
       </c>
       <c r="D17" s="1">
-        <v>0.1916542514218098</v>
+        <v>0.5877238379963322</v>
       </c>
       <c r="E17">
         <v>18</v>
@@ -1215,10 +1212,10 @@
         <v>10</v>
       </c>
       <c r="C18" s="1">
-        <v>0.5957613279533805</v>
+        <v>0.3166188715203264</v>
       </c>
       <c r="D18" s="1">
-        <v>0.2823111139439658</v>
+        <v>0.6950272937821849</v>
       </c>
       <c r="E18">
         <v>17</v>
@@ -1231,8 +1228,11 @@
       <c r="B19">
         <v>11</v>
       </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
       <c r="D19" s="1">
-        <v>0.1975815868176595</v>
+        <v>0.4799780978171799</v>
       </c>
       <c r="E19">
         <v>16</v>
@@ -1246,10 +1246,10 @@
         <v>12</v>
       </c>
       <c r="C20" s="1">
-        <v>0.7099376897136177</v>
+        <v>0.3676918970110236</v>
       </c>
       <c r="D20" s="1">
-        <v>0.113648553805877</v>
+        <v>0.4964041833034137</v>
       </c>
       <c r="E20">
         <v>15</v>
@@ -1263,10 +1263,10 @@
         <v>13</v>
       </c>
       <c r="C21" s="1">
-        <v>0.7725343881445893</v>
+        <v>0.5694399995102261</v>
       </c>
       <c r="D21" s="1">
-        <v>0.1971928126262711</v>
+        <v>0.4511452428471781</v>
       </c>
       <c r="E21">
         <v>14</v>
@@ -1280,10 +1280,10 @@
         <v>14</v>
       </c>
       <c r="C22" s="1">
-        <v>0.7534560635001963</v>
+        <v>0.6968909473354162</v>
       </c>
       <c r="D22" s="1">
-        <v>0.101893287078088</v>
+        <v>0.1808410096349255</v>
       </c>
       <c r="E22">
         <v>13</v>
@@ -1297,10 +1297,10 @@
         <v>15</v>
       </c>
       <c r="C23" s="1">
-        <v>0.9411399939792753</v>
+        <v>0.7322849197478155</v>
       </c>
       <c r="D23" s="1">
-        <v>0.03457147852972665</v>
+        <v>0.1557090277338459</v>
       </c>
       <c r="E23">
         <v>12</v>
@@ -1314,10 +1314,10 @@
         <v>16</v>
       </c>
       <c r="C24" s="1">
-        <v>0.8859485205328446</v>
+        <v>0.6805195656183084</v>
       </c>
       <c r="D24" s="1">
-        <v>0.06280325380231767</v>
+        <v>0.2110274212379415</v>
       </c>
       <c r="E24">
         <v>11</v>
@@ -1331,10 +1331,10 @@
         <v>17</v>
       </c>
       <c r="C25" s="1">
-        <v>0.9378870897892354</v>
+        <v>0.871710627973019</v>
       </c>
       <c r="D25" s="1">
-        <v>0</v>
+        <v>0.2286928381609282</v>
       </c>
       <c r="E25">
         <v>10</v>
@@ -1348,10 +1348,10 @@
         <v>18</v>
       </c>
       <c r="C26" s="1">
-        <v>0.9559561959853398</v>
+        <v>0.9542488324553626</v>
       </c>
       <c r="D26" s="1">
-        <v>0</v>
+        <v>0.044303539091117</v>
       </c>
       <c r="E26">
         <v>9</v>
@@ -1365,10 +1365,10 @@
         <v>19</v>
       </c>
       <c r="C27" s="1">
-        <v>0.9589717608419112</v>
+        <v>1</v>
       </c>
       <c r="D27" s="1">
-        <v>0</v>
+        <v>0.0865902006984151</v>
       </c>
       <c r="E27">
         <v>8</v>

</xml_diff>

<commit_message>
28.01.21 updated ion views, OccupancyRecalculator.py, ModellingTool.py, optimised multiprocessing
</commit_message>
<xml_diff>
--- a/Spectral_data/Occupancies_out.xlsx
+++ b/Spectral_data/Occupancies_out.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="11">
   <si>
-    <t>21/01/2021 17:01</t>
+    <t>28/01/2021 17:03</t>
   </si>
   <si>
     <t>fragmentation:</t>
@@ -237,83 +237,80 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
-                <c:pt idx="0">
+                <c:pt idx="1">
+                  <c:v>0.5235014664540886</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6711730973214913</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.682943575243352</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.4626587186933634</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.4205932279758092</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.6344577599912982</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.782280548001142</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.8647039252879164</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.9488675487083401</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.8698924878045139</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.9065769118955627</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.02619316325669712</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.1125775301471257</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.2504251496124864</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.5499320355782246</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.5778128800287456</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.7346830655264319</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.7821581879666387</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.8564513455232694</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.8506034105552747</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.9132174037202494</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.121284927433851</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.9636521959146575</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.002652910097581</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.142539564154538</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.382267183485992</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.24205398582156</c:v>
-                </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.378171875877741</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.497835779489556</c:v>
+                  <c:v>0.7079042506145522</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.554921524502883</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.495305756425543</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.765252599015753</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.422914804697499</c:v>
+                  <c:v>0.9525823130225165</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.942549381802448</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.899779617723811</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -801,9 +798,6 @@
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
       <c r="D8">
         <v>26</v>
       </c>
@@ -816,7 +810,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="1">
-        <v>0</v>
+        <v>0.5235014664540886</v>
       </c>
       <c r="D9">
         <v>25</v>
@@ -830,7 +824,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="1">
-        <v>0.02619316325669712</v>
+        <v>0</v>
       </c>
       <c r="D10">
         <v>24</v>
@@ -844,7 +838,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="1">
-        <v>0.1125775301471257</v>
+        <v>0</v>
       </c>
       <c r="D11">
         <v>23</v>
@@ -858,7 +852,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="1">
-        <v>0.2504251496124864</v>
+        <v>0</v>
       </c>
       <c r="D12">
         <v>22</v>
@@ -872,7 +866,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="1">
-        <v>0.5499320355782246</v>
+        <v>0</v>
       </c>
       <c r="D13">
         <v>21</v>
@@ -886,7 +880,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="1">
-        <v>0.5778128800287456</v>
+        <v>0.6711730973214913</v>
       </c>
       <c r="D14">
         <v>20</v>
@@ -900,7 +894,7 @@
         <v>8</v>
       </c>
       <c r="C15" s="1">
-        <v>0.7346830655264319</v>
+        <v>0.682943575243352</v>
       </c>
       <c r="D15">
         <v>19</v>
@@ -914,7 +908,7 @@
         <v>9</v>
       </c>
       <c r="C16" s="1">
-        <v>0.7821581879666387</v>
+        <v>0.4626587186933634</v>
       </c>
       <c r="D16">
         <v>18</v>
@@ -928,7 +922,7 @@
         <v>10</v>
       </c>
       <c r="C17" s="1">
-        <v>0.8564513455232694</v>
+        <v>0.4205932279758092</v>
       </c>
       <c r="D17">
         <v>17</v>
@@ -942,7 +936,7 @@
         <v>11</v>
       </c>
       <c r="C18" s="1">
-        <v>0.8506034105552747</v>
+        <v>0</v>
       </c>
       <c r="D18">
         <v>16</v>
@@ -956,7 +950,7 @@
         <v>12</v>
       </c>
       <c r="C19" s="1">
-        <v>0.9132174037202494</v>
+        <v>0.6344577599912982</v>
       </c>
       <c r="D19">
         <v>15</v>
@@ -970,7 +964,7 @@
         <v>13</v>
       </c>
       <c r="C20" s="1">
-        <v>1.121284927433851</v>
+        <v>0.782280548001142</v>
       </c>
       <c r="D20">
         <v>14</v>
@@ -984,7 +978,7 @@
         <v>14</v>
       </c>
       <c r="C21" s="1">
-        <v>0.9636521959146575</v>
+        <v>0.8647039252879164</v>
       </c>
       <c r="D21">
         <v>13</v>
@@ -998,7 +992,7 @@
         <v>15</v>
       </c>
       <c r="C22" s="1">
-        <v>1.002652910097581</v>
+        <v>0.9488675487083401</v>
       </c>
       <c r="D22">
         <v>12</v>
@@ -1012,7 +1006,7 @@
         <v>16</v>
       </c>
       <c r="C23" s="1">
-        <v>1.142539564154538</v>
+        <v>0.8698924878045139</v>
       </c>
       <c r="D23">
         <v>11</v>
@@ -1026,7 +1020,7 @@
         <v>17</v>
       </c>
       <c r="C24" s="1">
-        <v>1.382267183485992</v>
+        <v>0.9065769118955627</v>
       </c>
       <c r="D24">
         <v>10</v>
@@ -1040,7 +1034,7 @@
         <v>18</v>
       </c>
       <c r="C25" s="1">
-        <v>1.24205398582156</v>
+        <v>1</v>
       </c>
       <c r="D25">
         <v>9</v>
@@ -1054,7 +1048,7 @@
         <v>19</v>
       </c>
       <c r="C26" s="1">
-        <v>1.378171875877741</v>
+        <v>1</v>
       </c>
       <c r="D26">
         <v>8</v>
@@ -1068,7 +1062,7 @@
         <v>20</v>
       </c>
       <c r="C27" s="1">
-        <v>1.497835779489556</v>
+        <v>0.7079042506145522</v>
       </c>
       <c r="D27">
         <v>7</v>
@@ -1082,7 +1076,7 @@
         <v>21</v>
       </c>
       <c r="C28" s="1">
-        <v>1.554921524502883</v>
+        <v>1</v>
       </c>
       <c r="D28">
         <v>6</v>
@@ -1096,7 +1090,7 @@
         <v>22</v>
       </c>
       <c r="C29" s="1">
-        <v>1.495305756425543</v>
+        <v>1</v>
       </c>
       <c r="D29">
         <v>5</v>
@@ -1110,7 +1104,7 @@
         <v>23</v>
       </c>
       <c r="C30" s="1">
-        <v>1.765252599015753</v>
+        <v>1</v>
       </c>
       <c r="D30">
         <v>4</v>
@@ -1124,7 +1118,7 @@
         <v>24</v>
       </c>
       <c r="C31" s="1">
-        <v>1.422914804697499</v>
+        <v>0.9525823130225165</v>
       </c>
       <c r="D31">
         <v>3</v>
@@ -1138,7 +1132,7 @@
         <v>25</v>
       </c>
       <c r="C32" s="1">
-        <v>1.942549381802448</v>
+        <v>1</v>
       </c>
       <c r="D32">
         <v>2</v>
@@ -1152,7 +1146,7 @@
         <v>26</v>
       </c>
       <c r="C33" s="1">
-        <v>1.899779617723811</v>
+        <v>1</v>
       </c>
       <c r="D33">
         <v>1</v>

</xml_diff>

<commit_message>
25.03.21 debugging (overlaps are counted to int.(!), sorted ion lists when exporting, gui)
</commit_message>
<xml_diff>
--- a/Spectral_data/Occupancies_out.xlsx
+++ b/Spectral_data/Occupancies_out.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="12">
   <si>
-    <t>17/03/2021 19:44</t>
+    <t>25/03/2021 20:27</t>
   </si>
   <si>
     <t>fragmentation:</t>
@@ -256,40 +256,43 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.2948192554489688</c:v>
+                  <c:v>0.3365656838550645</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.3089824189933628</c:v>
+                  <c:v>0.3050197141048431</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.3091405136994379</c:v>
+                  <c:v>0.3564402734221735</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.3166188715203264</c:v>
+                  <c:v>0.3303662211294531</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.06836831387729592</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.3676918970110236</c:v>
+                  <c:v>0.4150792315697763</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.5694399995102261</c:v>
+                  <c:v>0.490932171481582</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.6968909473354162</c:v>
+                  <c:v>0.7611659124538951</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.7322849197478155</c:v>
+                  <c:v>0.7590097300531033</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.6805195656183084</c:v>
+                  <c:v>0.7407743094437484</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.871710627973019</c:v>
+                  <c:v>0.8831022467414469</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.9542488324553626</c:v>
+                  <c:v>0.9536766829963157</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1</c:v>
+                  <c:v>0.9314503605489437</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>1</c:v>
@@ -451,43 +454,46 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.9426793405802766</c:v>
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.5904833814888236</c:v>
+                  <c:v>0.507602598195334</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.5877238379963322</c:v>
+                  <c:v>0.478605129936724</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.6950272937821849</c:v>
+                  <c:v>0.5077904797018222</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.4799780978171799</c:v>
+                  <c:v>0.3561315541487868</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.4964041833034137</c:v>
+                  <c:v>0.4896803191695611</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.4511452428471781</c:v>
+                  <c:v>0.426321057237913</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.1808410096349255</c:v>
+                  <c:v>0.1447978060262054</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.1557090277338459</c:v>
+                  <c:v>0.1071137301099014</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.2110274212379415</c:v>
+                  <c:v>0.1530169980103788</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.2286928381609282</c:v>
+                  <c:v>0.09766664629868996</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.044303539091117</c:v>
+                  <c:v>0.008770758953145222</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.0865902006984151</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
@@ -1021,7 +1027,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>0.4578146032106267</v>
+        <v>0.4503119129516114</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1029,7 +1035,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>0.5421853967893733</v>
+        <v>0.5496880870483885</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1147,7 +1153,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="1">
-        <v>0.9426793405802766</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <v>21</v>
@@ -1161,7 +1167,10 @@
         <v>7</v>
       </c>
       <c r="C15" s="1">
-        <v>0.2948192554489688</v>
+        <v>0.3365656838550645</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
       </c>
       <c r="E15">
         <v>20</v>
@@ -1175,10 +1184,10 @@
         <v>8</v>
       </c>
       <c r="C16" s="1">
-        <v>0.3089824189933628</v>
+        <v>0.3050197141048431</v>
       </c>
       <c r="D16" s="1">
-        <v>0.5904833814888236</v>
+        <v>0.507602598195334</v>
       </c>
       <c r="E16">
         <v>19</v>
@@ -1192,10 +1201,10 @@
         <v>9</v>
       </c>
       <c r="C17" s="1">
-        <v>0.3091405136994379</v>
+        <v>0.3564402734221735</v>
       </c>
       <c r="D17" s="1">
-        <v>0.5877238379963322</v>
+        <v>0.478605129936724</v>
       </c>
       <c r="E17">
         <v>18</v>
@@ -1209,10 +1218,10 @@
         <v>10</v>
       </c>
       <c r="C18" s="1">
-        <v>0.3166188715203264</v>
+        <v>0.3303662211294531</v>
       </c>
       <c r="D18" s="1">
-        <v>0.6950272937821849</v>
+        <v>0.5077904797018222</v>
       </c>
       <c r="E18">
         <v>17</v>
@@ -1225,8 +1234,11 @@
       <c r="B19">
         <v>11</v>
       </c>
+      <c r="C19" s="1">
+        <v>0.06836831387729592</v>
+      </c>
       <c r="D19" s="1">
-        <v>0.4799780978171799</v>
+        <v>0.3561315541487868</v>
       </c>
       <c r="E19">
         <v>16</v>
@@ -1240,10 +1252,10 @@
         <v>12</v>
       </c>
       <c r="C20" s="1">
-        <v>0.3676918970110236</v>
+        <v>0.4150792315697763</v>
       </c>
       <c r="D20" s="1">
-        <v>0.4964041833034137</v>
+        <v>0.4896803191695611</v>
       </c>
       <c r="E20">
         <v>15</v>
@@ -1257,10 +1269,10 @@
         <v>13</v>
       </c>
       <c r="C21" s="1">
-        <v>0.5694399995102261</v>
+        <v>0.490932171481582</v>
       </c>
       <c r="D21" s="1">
-        <v>0.4511452428471781</v>
+        <v>0.426321057237913</v>
       </c>
       <c r="E21">
         <v>14</v>
@@ -1274,10 +1286,10 @@
         <v>14</v>
       </c>
       <c r="C22" s="1">
-        <v>0.6968909473354162</v>
+        <v>0.7611659124538951</v>
       </c>
       <c r="D22" s="1">
-        <v>0.1808410096349255</v>
+        <v>0.1447978060262054</v>
       </c>
       <c r="E22">
         <v>13</v>
@@ -1291,10 +1303,10 @@
         <v>15</v>
       </c>
       <c r="C23" s="1">
-        <v>0.7322849197478155</v>
+        <v>0.7590097300531033</v>
       </c>
       <c r="D23" s="1">
-        <v>0.1557090277338459</v>
+        <v>0.1071137301099014</v>
       </c>
       <c r="E23">
         <v>12</v>
@@ -1308,10 +1320,10 @@
         <v>16</v>
       </c>
       <c r="C24" s="1">
-        <v>0.6805195656183084</v>
+        <v>0.7407743094437484</v>
       </c>
       <c r="D24" s="1">
-        <v>0.2110274212379415</v>
+        <v>0.1530169980103788</v>
       </c>
       <c r="E24">
         <v>11</v>
@@ -1325,10 +1337,10 @@
         <v>17</v>
       </c>
       <c r="C25" s="1">
-        <v>0.871710627973019</v>
+        <v>0.8831022467414469</v>
       </c>
       <c r="D25" s="1">
-        <v>0.2286928381609282</v>
+        <v>0.09766664629868996</v>
       </c>
       <c r="E25">
         <v>10</v>
@@ -1342,10 +1354,10 @@
         <v>18</v>
       </c>
       <c r="C26" s="1">
-        <v>0.9542488324553626</v>
+        <v>0.9536766829963157</v>
       </c>
       <c r="D26" s="1">
-        <v>0.044303539091117</v>
+        <v>0.008770758953145222</v>
       </c>
       <c r="E26">
         <v>9</v>
@@ -1359,10 +1371,10 @@
         <v>19</v>
       </c>
       <c r="C27" s="1">
-        <v>1</v>
+        <v>0.9314503605489437</v>
       </c>
       <c r="D27" s="1">
-        <v>0.0865902006984151</v>
+        <v>0</v>
       </c>
       <c r="E27">
         <v>8</v>

</xml_diff>

<commit_message>
01.04.21 debugging (copying peak table)
</commit_message>
<xml_diff>
--- a/Spectral_data/Occupancies_out.xlsx
+++ b/Spectral_data/Occupancies_out.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="12">
   <si>
-    <t>25/03/2021 20:27</t>
+    <t>01/04/2021 11:01</t>
   </si>
   <si>
     <t>fragmentation:</t>
@@ -253,46 +253,43 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.02000087177686502</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.3365656838550645</c:v>
+                  <c:v>0.3351697413725013</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.3050197141048431</c:v>
+                  <c:v>0.4721014773042254</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.3564402734221735</c:v>
+                  <c:v>0.3554065646873324</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.3303662211294531</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.06836831387729592</c:v>
+                  <c:v>0.4234487810123325</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.4150792315697763</c:v>
+                  <c:v>0.4358916870624788</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.490932171481582</c:v>
+                  <c:v>0.5452501465705899</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.7611659124538951</c:v>
+                  <c:v>0.7626031934592458</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.7590097300531033</c:v>
+                  <c:v>0.8227067731027261</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.7407743094437484</c:v>
+                  <c:v>0.7303401947315076</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.8831022467414469</c:v>
+                  <c:v>0.8954395298949853</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.9536766829963157</c:v>
+                  <c:v>0.9253528371680027</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.9314503605489437</c:v>
+                  <c:v>0.941606353845397</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>1</c:v>
@@ -456,44 +453,41 @@
                 <c:pt idx="5">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.507602598195334</c:v>
+                  <c:v>0.4600179281589262</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.478605129936724</c:v>
+                  <c:v>0.5027834654089542</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.5077904797018222</c:v>
+                  <c:v>0.5317488919926445</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.3561315541487868</c:v>
+                  <c:v>0.4371745787899363</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.4896803191695611</c:v>
+                  <c:v>0.4689236312318184</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.426321057237913</c:v>
+                  <c:v>0.3813157300431642</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.1447978060262054</c:v>
+                  <c:v>0.2165900832457863</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.1071137301099014</c:v>
+                  <c:v>0.1274002410339445</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.1530169980103788</c:v>
+                  <c:v>0.2021415448718557</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.09766664629868996</c:v>
+                  <c:v>0.1289371743655314</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.008770758953145222</c:v>
+                  <c:v>0.0327568583004501</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>0.01807710150318315</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
@@ -1027,7 +1021,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>0.4503119129516114</v>
+        <v>0.4615051419869385</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1035,7 +1029,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>0.5496880870483885</v>
+        <v>0.5384948580130613</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1150,7 +1144,7 @@
         <v>6</v>
       </c>
       <c r="C14" s="1">
-        <v>0</v>
+        <v>0.02000087177686502</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
@@ -1167,10 +1161,7 @@
         <v>7</v>
       </c>
       <c r="C15" s="1">
-        <v>0.3365656838550645</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1</v>
+        <v>0.3351697413725013</v>
       </c>
       <c r="E15">
         <v>20</v>
@@ -1184,10 +1175,10 @@
         <v>8</v>
       </c>
       <c r="C16" s="1">
-        <v>0.3050197141048431</v>
+        <v>0.4721014773042254</v>
       </c>
       <c r="D16" s="1">
-        <v>0.507602598195334</v>
+        <v>0.4600179281589262</v>
       </c>
       <c r="E16">
         <v>19</v>
@@ -1201,10 +1192,10 @@
         <v>9</v>
       </c>
       <c r="C17" s="1">
-        <v>0.3564402734221735</v>
+        <v>0.3554065646873324</v>
       </c>
       <c r="D17" s="1">
-        <v>0.478605129936724</v>
+        <v>0.5027834654089542</v>
       </c>
       <c r="E17">
         <v>18</v>
@@ -1218,10 +1209,10 @@
         <v>10</v>
       </c>
       <c r="C18" s="1">
-        <v>0.3303662211294531</v>
+        <v>0.4234487810123325</v>
       </c>
       <c r="D18" s="1">
-        <v>0.5077904797018222</v>
+        <v>0.5317488919926445</v>
       </c>
       <c r="E18">
         <v>17</v>
@@ -1234,11 +1225,8 @@
       <c r="B19">
         <v>11</v>
       </c>
-      <c r="C19" s="1">
-        <v>0.06836831387729592</v>
-      </c>
       <c r="D19" s="1">
-        <v>0.3561315541487868</v>
+        <v>0.4371745787899363</v>
       </c>
       <c r="E19">
         <v>16</v>
@@ -1252,10 +1240,10 @@
         <v>12</v>
       </c>
       <c r="C20" s="1">
-        <v>0.4150792315697763</v>
+        <v>0.4358916870624788</v>
       </c>
       <c r="D20" s="1">
-        <v>0.4896803191695611</v>
+        <v>0.4689236312318184</v>
       </c>
       <c r="E20">
         <v>15</v>
@@ -1269,10 +1257,10 @@
         <v>13</v>
       </c>
       <c r="C21" s="1">
-        <v>0.490932171481582</v>
+        <v>0.5452501465705899</v>
       </c>
       <c r="D21" s="1">
-        <v>0.426321057237913</v>
+        <v>0.3813157300431642</v>
       </c>
       <c r="E21">
         <v>14</v>
@@ -1286,10 +1274,10 @@
         <v>14</v>
       </c>
       <c r="C22" s="1">
-        <v>0.7611659124538951</v>
+        <v>0.7626031934592458</v>
       </c>
       <c r="D22" s="1">
-        <v>0.1447978060262054</v>
+        <v>0.2165900832457863</v>
       </c>
       <c r="E22">
         <v>13</v>
@@ -1303,10 +1291,10 @@
         <v>15</v>
       </c>
       <c r="C23" s="1">
-        <v>0.7590097300531033</v>
+        <v>0.8227067731027261</v>
       </c>
       <c r="D23" s="1">
-        <v>0.1071137301099014</v>
+        <v>0.1274002410339445</v>
       </c>
       <c r="E23">
         <v>12</v>
@@ -1320,10 +1308,10 @@
         <v>16</v>
       </c>
       <c r="C24" s="1">
-        <v>0.7407743094437484</v>
+        <v>0.7303401947315076</v>
       </c>
       <c r="D24" s="1">
-        <v>0.1530169980103788</v>
+        <v>0.2021415448718557</v>
       </c>
       <c r="E24">
         <v>11</v>
@@ -1337,10 +1325,10 @@
         <v>17</v>
       </c>
       <c r="C25" s="1">
-        <v>0.8831022467414469</v>
+        <v>0.8954395298949853</v>
       </c>
       <c r="D25" s="1">
-        <v>0.09766664629868996</v>
+        <v>0.1289371743655314</v>
       </c>
       <c r="E25">
         <v>10</v>
@@ -1354,10 +1342,10 @@
         <v>18</v>
       </c>
       <c r="C26" s="1">
-        <v>0.9536766829963157</v>
+        <v>0.9253528371680027</v>
       </c>
       <c r="D26" s="1">
-        <v>0.008770758953145222</v>
+        <v>0.0327568583004501</v>
       </c>
       <c r="E26">
         <v>9</v>
@@ -1371,10 +1359,10 @@
         <v>19</v>
       </c>
       <c r="C27" s="1">
-        <v>0.9314503605489437</v>
+        <v>0.941606353845397</v>
       </c>
       <c r="D27" s="1">
-        <v>0</v>
+        <v>0.01807710150318315</v>
       </c>
       <c r="E27">
         <v>8</v>

</xml_diff>

<commit_message>
02.04.21 cleaning folder structure
</commit_message>
<xml_diff>
--- a/Spectral_data/Occupancies_out.xlsx
+++ b/Spectral_data/Occupancies_out.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="12">
   <si>
-    <t>01/04/2021 11:01</t>
+    <t>02/04/2021 11:46</t>
   </si>
   <si>
     <t>fragmentation:</t>
@@ -253,43 +253,43 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.02000087177686502</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.3351697413725013</c:v>
+                  <c:v>0.6499526708767375</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.4721014773042254</c:v>
+                  <c:v>0.679930242599976</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.3554065646873324</c:v>
+                  <c:v>0.7347938574539591</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.4234487810123325</c:v>
+                  <c:v>0.5177154407963372</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.4358916870624788</c:v>
+                  <c:v>0.6854190159458917</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.5452501465705899</c:v>
+                  <c:v>0.7877297936304034</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.7626031934592458</c:v>
+                  <c:v>0.8523740931847611</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.8227067731027261</c:v>
+                  <c:v>0.9436683563245826</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.7303401947315076</c:v>
+                  <c:v>0.895664937390644</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.8954395298949853</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.9253528371680027</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.941606353845397</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>1</c:v>
@@ -454,40 +454,40 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.4600179281589262</c:v>
+                  <c:v>0.227608881117836</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.5027834654089542</c:v>
+                  <c:v>0.2427359598426374</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.5317488919926445</c:v>
+                  <c:v>0.3079322317258981</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.4371745787899363</c:v>
+                  <c:v>0.2489940375985687</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.4689236312318184</c:v>
+                  <c:v>0.2181330311580482</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.3813157300431642</c:v>
+                  <c:v>0.1894773278565225</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.2165900832457863</c:v>
+                  <c:v>0.106548904989473</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.1274002410339445</c:v>
+                  <c:v>0.01490999286018015</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.2021415448718557</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.1289371743655314</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.0327568583004501</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.01807710150318315</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
@@ -1021,7 +1021,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>0.4615051419869385</v>
+        <v>0.4326052928353927</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1029,7 +1029,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>0.5384948580130613</v>
+        <v>0.5673947071646074</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1144,7 +1144,7 @@
         <v>6</v>
       </c>
       <c r="C14" s="1">
-        <v>0.02000087177686502</v>
+        <v>0</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
@@ -1161,7 +1161,7 @@
         <v>7</v>
       </c>
       <c r="C15" s="1">
-        <v>0.3351697413725013</v>
+        <v>0.6499526708767375</v>
       </c>
       <c r="E15">
         <v>20</v>
@@ -1175,10 +1175,10 @@
         <v>8</v>
       </c>
       <c r="C16" s="1">
-        <v>0.4721014773042254</v>
+        <v>0.679930242599976</v>
       </c>
       <c r="D16" s="1">
-        <v>0.4600179281589262</v>
+        <v>0.227608881117836</v>
       </c>
       <c r="E16">
         <v>19</v>
@@ -1192,10 +1192,10 @@
         <v>9</v>
       </c>
       <c r="C17" s="1">
-        <v>0.3554065646873324</v>
+        <v>0.7347938574539591</v>
       </c>
       <c r="D17" s="1">
-        <v>0.5027834654089542</v>
+        <v>0.2427359598426374</v>
       </c>
       <c r="E17">
         <v>18</v>
@@ -1209,10 +1209,10 @@
         <v>10</v>
       </c>
       <c r="C18" s="1">
-        <v>0.4234487810123325</v>
+        <v>0.5177154407963372</v>
       </c>
       <c r="D18" s="1">
-        <v>0.5317488919926445</v>
+        <v>0.3079322317258981</v>
       </c>
       <c r="E18">
         <v>17</v>
@@ -1226,7 +1226,7 @@
         <v>11</v>
       </c>
       <c r="D19" s="1">
-        <v>0.4371745787899363</v>
+        <v>0.2489940375985687</v>
       </c>
       <c r="E19">
         <v>16</v>
@@ -1240,10 +1240,10 @@
         <v>12</v>
       </c>
       <c r="C20" s="1">
-        <v>0.4358916870624788</v>
+        <v>0.6854190159458917</v>
       </c>
       <c r="D20" s="1">
-        <v>0.4689236312318184</v>
+        <v>0.2181330311580482</v>
       </c>
       <c r="E20">
         <v>15</v>
@@ -1257,10 +1257,10 @@
         <v>13</v>
       </c>
       <c r="C21" s="1">
-        <v>0.5452501465705899</v>
+        <v>0.7877297936304034</v>
       </c>
       <c r="D21" s="1">
-        <v>0.3813157300431642</v>
+        <v>0.1894773278565225</v>
       </c>
       <c r="E21">
         <v>14</v>
@@ -1274,10 +1274,10 @@
         <v>14</v>
       </c>
       <c r="C22" s="1">
-        <v>0.7626031934592458</v>
+        <v>0.8523740931847611</v>
       </c>
       <c r="D22" s="1">
-        <v>0.2165900832457863</v>
+        <v>0.106548904989473</v>
       </c>
       <c r="E22">
         <v>13</v>
@@ -1291,10 +1291,10 @@
         <v>15</v>
       </c>
       <c r="C23" s="1">
-        <v>0.8227067731027261</v>
+        <v>0.9436683563245826</v>
       </c>
       <c r="D23" s="1">
-        <v>0.1274002410339445</v>
+        <v>0.01490999286018015</v>
       </c>
       <c r="E23">
         <v>12</v>
@@ -1308,10 +1308,10 @@
         <v>16</v>
       </c>
       <c r="C24" s="1">
-        <v>0.7303401947315076</v>
+        <v>0.895664937390644</v>
       </c>
       <c r="D24" s="1">
-        <v>0.2021415448718557</v>
+        <v>0</v>
       </c>
       <c r="E24">
         <v>11</v>
@@ -1325,10 +1325,10 @@
         <v>17</v>
       </c>
       <c r="C25" s="1">
-        <v>0.8954395298949853</v>
+        <v>1</v>
       </c>
       <c r="D25" s="1">
-        <v>0.1289371743655314</v>
+        <v>0</v>
       </c>
       <c r="E25">
         <v>10</v>
@@ -1342,10 +1342,10 @@
         <v>18</v>
       </c>
       <c r="C26" s="1">
-        <v>0.9253528371680027</v>
+        <v>1</v>
       </c>
       <c r="D26" s="1">
-        <v>0.0327568583004501</v>
+        <v>0</v>
       </c>
       <c r="E26">
         <v>9</v>
@@ -1359,10 +1359,10 @@
         <v>19</v>
       </c>
       <c r="C27" s="1">
-        <v>0.941606353845397</v>
+        <v>1</v>
       </c>
       <c r="D27" s="1">
-        <v>0.01807710150318315</v>
+        <v>0</v>
       </c>
       <c r="E27">
         <v>8</v>

</xml_diff>

<commit_message>
13.04.21 debugging (IsoPatternPeakView: copying table, OccupancyRecalculator.py: loading Occupancies_in.csv)
</commit_message>
<xml_diff>
--- a/Spectral_data/Occupancies_out.xlsx
+++ b/Spectral_data/Occupancies_out.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="12">
   <si>
-    <t>02/04/2021 11:46</t>
+    <t>13/04/2021 17:39</t>
   </si>
   <si>
     <t>fragmentation:</t>
@@ -244,73 +244,70 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.1724538867617657</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>0.09128218680418146</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.08061230026340492</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.1229420682206724</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1235458202654845</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.6499526708767375</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.679930242599976</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.7347938574539591</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.5177154407963372</c:v>
+                  <c:v>0.0735704151443306</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.6854190159458917</c:v>
+                  <c:v>0.5621945415081315</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.7877297936304034</c:v>
+                  <c:v>0.1809350292162644</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.8523740931847611</c:v>
+                  <c:v>0.1636447119069271</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.9436683563245826</c:v>
+                  <c:v>0.1381611054857339</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.895664937390644</c:v>
+                  <c:v>0.2282825262821861</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1</c:v>
+                  <c:v>0.2276192464347997</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1</c:v>
+                  <c:v>0.3663844860194911</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1</c:v>
+                  <c:v>0.3652077072120486</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1</c:v>
+                  <c:v>0.4065624587608148</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1</c:v>
+                  <c:v>0.3750525719654789</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1</c:v>
+                  <c:v>0.402773541720006</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1</c:v>
+                  <c:v>0.4116730285605797</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1</c:v>
+                  <c:v>0.2284720697855734</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1</c:v>
+                  <c:v>0.4324044374920852</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -436,76 +433,79 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.9702968525780499</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0.859310439376442</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0.9002876039349853</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0.952367657234294</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0.9089060143233461</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8096547457916253</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8748118411885112</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.90816800837282</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.8253846146228404</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.227608881117836</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.2427359598426374</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.3079322317258981</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.2489940375985687</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.2181330311580482</c:v>
+                  <c:v>0.7748609036594906</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.1894773278565225</c:v>
+                  <c:v>0.8123476569107348</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.106548904989473</c:v>
+                  <c:v>0.8059151036038091</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.01490999286018015</c:v>
+                  <c:v>0.7574638473677997</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>0.8170294457232519</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>0.7904972105057587</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>0.6868570095767319</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>0.678462449211344</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>0.7349813382823553</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>0.6364863328227983</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>0.7398683720896356</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>0.7322917929956112</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>0.6812152183654794</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>0.6872980780634957</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1021,7 +1021,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>0.4326052928353927</v>
+        <v>0.4967469870553322</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1029,7 +1029,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>0.5673947071646074</v>
+        <v>0.5032530129446677</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1062,7 +1062,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="1">
-        <v>1</v>
+        <v>0.9702968525780499</v>
       </c>
       <c r="E9">
         <v>26</v>
@@ -1079,7 +1079,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="1">
-        <v>1</v>
+        <v>0.859310439376442</v>
       </c>
       <c r="E10">
         <v>25</v>
@@ -1093,10 +1093,10 @@
         <v>3</v>
       </c>
       <c r="C11" s="1">
-        <v>0</v>
+        <v>0.1724538867617657</v>
       </c>
       <c r="D11" s="1">
-        <v>1</v>
+        <v>0.9002876039349853</v>
       </c>
       <c r="E11">
         <v>24</v>
@@ -1113,7 +1113,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="1">
-        <v>1</v>
+        <v>0.952367657234294</v>
       </c>
       <c r="E12">
         <v>23</v>
@@ -1127,7 +1127,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="1">
-        <v>0</v>
+        <v>0.09128218680418146</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
@@ -1144,10 +1144,10 @@
         <v>6</v>
       </c>
       <c r="C14" s="1">
-        <v>0</v>
+        <v>0.08061230026340492</v>
       </c>
       <c r="D14" s="1">
-        <v>1</v>
+        <v>0.9089060143233461</v>
       </c>
       <c r="E14">
         <v>21</v>
@@ -1161,7 +1161,10 @@
         <v>7</v>
       </c>
       <c r="C15" s="1">
-        <v>0.6499526708767375</v>
+        <v>0.1229420682206724</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.8096547457916253</v>
       </c>
       <c r="E15">
         <v>20</v>
@@ -1175,10 +1178,10 @@
         <v>8</v>
       </c>
       <c r="C16" s="1">
-        <v>0.679930242599976</v>
+        <v>0.1235458202654845</v>
       </c>
       <c r="D16" s="1">
-        <v>0.227608881117836</v>
+        <v>0.8748118411885112</v>
       </c>
       <c r="E16">
         <v>19</v>
@@ -1192,10 +1195,10 @@
         <v>9</v>
       </c>
       <c r="C17" s="1">
-        <v>0.7347938574539591</v>
+        <v>0</v>
       </c>
       <c r="D17" s="1">
-        <v>0.2427359598426374</v>
+        <v>0.90816800837282</v>
       </c>
       <c r="E17">
         <v>18</v>
@@ -1209,10 +1212,10 @@
         <v>10</v>
       </c>
       <c r="C18" s="1">
-        <v>0.5177154407963372</v>
+        <v>0.0735704151443306</v>
       </c>
       <c r="D18" s="1">
-        <v>0.3079322317258981</v>
+        <v>0.8253846146228404</v>
       </c>
       <c r="E18">
         <v>17</v>
@@ -1226,7 +1229,7 @@
         <v>11</v>
       </c>
       <c r="D19" s="1">
-        <v>0.2489940375985687</v>
+        <v>1</v>
       </c>
       <c r="E19">
         <v>16</v>
@@ -1240,10 +1243,10 @@
         <v>12</v>
       </c>
       <c r="C20" s="1">
-        <v>0.6854190159458917</v>
+        <v>0.5621945415081315</v>
       </c>
       <c r="D20" s="1">
-        <v>0.2181330311580482</v>
+        <v>0.7748609036594906</v>
       </c>
       <c r="E20">
         <v>15</v>
@@ -1257,10 +1260,10 @@
         <v>13</v>
       </c>
       <c r="C21" s="1">
-        <v>0.7877297936304034</v>
+        <v>0.1809350292162644</v>
       </c>
       <c r="D21" s="1">
-        <v>0.1894773278565225</v>
+        <v>0.8123476569107348</v>
       </c>
       <c r="E21">
         <v>14</v>
@@ -1274,10 +1277,10 @@
         <v>14</v>
       </c>
       <c r="C22" s="1">
-        <v>0.8523740931847611</v>
+        <v>0.1636447119069271</v>
       </c>
       <c r="D22" s="1">
-        <v>0.106548904989473</v>
+        <v>0.8059151036038091</v>
       </c>
       <c r="E22">
         <v>13</v>
@@ -1291,10 +1294,10 @@
         <v>15</v>
       </c>
       <c r="C23" s="1">
-        <v>0.9436683563245826</v>
+        <v>0.1381611054857339</v>
       </c>
       <c r="D23" s="1">
-        <v>0.01490999286018015</v>
+        <v>0.7574638473677997</v>
       </c>
       <c r="E23">
         <v>12</v>
@@ -1308,10 +1311,10 @@
         <v>16</v>
       </c>
       <c r="C24" s="1">
-        <v>0.895664937390644</v>
+        <v>0.2282825262821861</v>
       </c>
       <c r="D24" s="1">
-        <v>0</v>
+        <v>0.8170294457232519</v>
       </c>
       <c r="E24">
         <v>11</v>
@@ -1325,10 +1328,10 @@
         <v>17</v>
       </c>
       <c r="C25" s="1">
-        <v>1</v>
+        <v>0.2276192464347997</v>
       </c>
       <c r="D25" s="1">
-        <v>0</v>
+        <v>0.7904972105057587</v>
       </c>
       <c r="E25">
         <v>10</v>
@@ -1342,10 +1345,10 @@
         <v>18</v>
       </c>
       <c r="C26" s="1">
-        <v>1</v>
+        <v>0.3663844860194911</v>
       </c>
       <c r="D26" s="1">
-        <v>0</v>
+        <v>0.6868570095767319</v>
       </c>
       <c r="E26">
         <v>9</v>
@@ -1359,10 +1362,10 @@
         <v>19</v>
       </c>
       <c r="C27" s="1">
-        <v>1</v>
+        <v>0.3652077072120486</v>
       </c>
       <c r="D27" s="1">
-        <v>0</v>
+        <v>0.678462449211344</v>
       </c>
       <c r="E27">
         <v>8</v>
@@ -1376,10 +1379,10 @@
         <v>20</v>
       </c>
       <c r="C28" s="1">
-        <v>1</v>
+        <v>0.4065624587608148</v>
       </c>
       <c r="D28" s="1">
-        <v>0</v>
+        <v>0.7349813382823553</v>
       </c>
       <c r="E28">
         <v>7</v>
@@ -1393,10 +1396,10 @@
         <v>21</v>
       </c>
       <c r="C29" s="1">
-        <v>1</v>
+        <v>0.3750525719654789</v>
       </c>
       <c r="D29" s="1">
-        <v>0</v>
+        <v>0.6364863328227983</v>
       </c>
       <c r="E29">
         <v>6</v>
@@ -1410,10 +1413,10 @@
         <v>22</v>
       </c>
       <c r="C30" s="1">
-        <v>1</v>
+        <v>0.402773541720006</v>
       </c>
       <c r="D30" s="1">
-        <v>0</v>
+        <v>0.7398683720896356</v>
       </c>
       <c r="E30">
         <v>5</v>
@@ -1427,10 +1430,10 @@
         <v>23</v>
       </c>
       <c r="C31" s="1">
-        <v>1</v>
+        <v>0.4116730285605797</v>
       </c>
       <c r="D31" s="1">
-        <v>0</v>
+        <v>0.7322917929956112</v>
       </c>
       <c r="E31">
         <v>4</v>
@@ -1444,10 +1447,10 @@
         <v>24</v>
       </c>
       <c r="C32" s="1">
-        <v>1</v>
+        <v>0.2284720697855734</v>
       </c>
       <c r="D32" s="1">
-        <v>0</v>
+        <v>0.6812152183654794</v>
       </c>
       <c r="E32">
         <v>3</v>
@@ -1461,10 +1464,10 @@
         <v>25</v>
       </c>
       <c r="C33" s="1">
-        <v>1</v>
+        <v>0.4324044374920852</v>
       </c>
       <c r="D33" s="1">
-        <v>0</v>
+        <v>0.6872980780634957</v>
       </c>
       <c r="E33">
         <v>2</v>
@@ -1476,9 +1479,6 @@
       </c>
       <c r="B34">
         <v>26</v>
-      </c>
-      <c r="C34" s="1">
-        <v>1</v>
       </c>
       <c r="E34">
         <v>1</v>

</xml_diff>

<commit_message>
15.07.21 Finished export options
</commit_message>
<xml_diff>
--- a/Spectral_data/Occupancies_out.xlsx
+++ b/Spectral_data/Occupancies_out.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="12">
   <si>
-    <t>13/04/2021 17:39</t>
+    <t>16/07/2021 09:26</t>
   </si>
   <si>
     <t>fragmentation:</t>
@@ -244,70 +244,76 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1724538867617657</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.09128218680418146</c:v>
+                  <c:v>0.1824670653632344</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.08061230026340492</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.1229420682206724</c:v>
+                  <c:v>0.3713393219524556</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.1235458202654845</c:v>
+                  <c:v>0.4524467626064254</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>0.297255549154257</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.4311368899685053</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.0735704151443306</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.5621945415081315</c:v>
+                  <c:v>0.435889064979885</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.1809350292162644</c:v>
+                  <c:v>0.5452539943146544</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.1636447119069271</c:v>
+                  <c:v>0.7656993893382078</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.1381611054857339</c:v>
+                  <c:v>0.8346920127058352</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.2282825262821861</c:v>
+                  <c:v>0.7274706849640297</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.2276192464347997</c:v>
+                  <c:v>0.9096400134282258</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.3663844860194911</c:v>
+                  <c:v>0.9261676110347306</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.3652077072120486</c:v>
+                  <c:v>0.9453144100552824</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.4065624587608148</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.3750525719654789</c:v>
+                  <c:v>0.9795071410359218</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.402773541720006</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.4116730285605797</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.2284720697855734</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.4324044374920852</c:v>
+                  <c:v>0.9757517052346958</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -433,79 +439,79 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>0.9702968525780499</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.859310439376442</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.9002876039349853</c:v>
+                  <c:v>0.04088863556810497</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.952367657234294</c:v>
+                  <c:v>0.775330355050239</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.9089060143233461</c:v>
+                  <c:v>0.8701710938353409</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.8096547457916253</c:v>
+                  <c:v>0.6350668206904492</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.8748118411885112</c:v>
+                  <c:v>0.4409841597897683</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.90816800837282</c:v>
+                  <c:v>0.5690547461769253</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.8253846146228404</c:v>
+                  <c:v>0.6599488907230143</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>0.4150167147834023</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.7748609036594906</c:v>
+                  <c:v>0.4733584948958165</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.8123476569107348</c:v>
+                  <c:v>0.3730859340305037</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.8059151036038091</c:v>
+                  <c:v>0.1988705560760465</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.7574638473677997</c:v>
+                  <c:v>0.1406221465654954</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.8170294457232519</c:v>
+                  <c:v>0.188223641739365</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.7904972105057587</c:v>
+                  <c:v>0.10753769620323</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.6868570095767319</c:v>
+                  <c:v>0.031986823289332</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.678462449211344</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.7349813382823553</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.6364863328227983</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.7398683720896356</c:v>
+                  <c:v>0.09827170168442574</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.7322917929956112</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.6812152183654794</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.6872980780634957</c:v>
+                  <c:v>0.03600326541959095</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1021,7 +1027,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>0.4967469870553322</v>
+        <v>0.3746581944490083</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1029,7 +1035,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>0.5032530129446677</v>
+        <v>0.6253418055509914</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1062,7 +1068,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="1">
-        <v>0.9702968525780499</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <v>26</v>
@@ -1079,7 +1085,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="1">
-        <v>0.859310439376442</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <v>25</v>
@@ -1093,10 +1099,10 @@
         <v>3</v>
       </c>
       <c r="C11" s="1">
-        <v>0.1724538867617657</v>
+        <v>0</v>
       </c>
       <c r="D11" s="1">
-        <v>0.9002876039349853</v>
+        <v>0.04088863556810497</v>
       </c>
       <c r="E11">
         <v>24</v>
@@ -1113,7 +1119,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="1">
-        <v>0.952367657234294</v>
+        <v>0.775330355050239</v>
       </c>
       <c r="E12">
         <v>23</v>
@@ -1127,7 +1133,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="1">
-        <v>0.09128218680418146</v>
+        <v>0.1824670653632344</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
@@ -1144,10 +1150,10 @@
         <v>6</v>
       </c>
       <c r="C14" s="1">
-        <v>0.08061230026340492</v>
+        <v>0</v>
       </c>
       <c r="D14" s="1">
-        <v>0.9089060143233461</v>
+        <v>0.8701710938353409</v>
       </c>
       <c r="E14">
         <v>21</v>
@@ -1161,10 +1167,10 @@
         <v>7</v>
       </c>
       <c r="C15" s="1">
-        <v>0.1229420682206724</v>
+        <v>0.3713393219524556</v>
       </c>
       <c r="D15" s="1">
-        <v>0.8096547457916253</v>
+        <v>0.6350668206904492</v>
       </c>
       <c r="E15">
         <v>20</v>
@@ -1178,10 +1184,10 @@
         <v>8</v>
       </c>
       <c r="C16" s="1">
-        <v>0.1235458202654845</v>
+        <v>0.4524467626064254</v>
       </c>
       <c r="D16" s="1">
-        <v>0.8748118411885112</v>
+        <v>0.4409841597897683</v>
       </c>
       <c r="E16">
         <v>19</v>
@@ -1195,10 +1201,10 @@
         <v>9</v>
       </c>
       <c r="C17" s="1">
-        <v>0</v>
+        <v>0.297255549154257</v>
       </c>
       <c r="D17" s="1">
-        <v>0.90816800837282</v>
+        <v>0.5690547461769253</v>
       </c>
       <c r="E17">
         <v>18</v>
@@ -1212,10 +1218,10 @@
         <v>10</v>
       </c>
       <c r="C18" s="1">
-        <v>0.0735704151443306</v>
+        <v>0.4311368899685053</v>
       </c>
       <c r="D18" s="1">
-        <v>0.8253846146228404</v>
+        <v>0.6599488907230143</v>
       </c>
       <c r="E18">
         <v>17</v>
@@ -1228,8 +1234,11 @@
       <c r="B19">
         <v>11</v>
       </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
       <c r="D19" s="1">
-        <v>1</v>
+        <v>0.4150167147834023</v>
       </c>
       <c r="E19">
         <v>16</v>
@@ -1243,10 +1252,10 @@
         <v>12</v>
       </c>
       <c r="C20" s="1">
-        <v>0.5621945415081315</v>
+        <v>0.435889064979885</v>
       </c>
       <c r="D20" s="1">
-        <v>0.7748609036594906</v>
+        <v>0.4733584948958165</v>
       </c>
       <c r="E20">
         <v>15</v>
@@ -1260,10 +1269,10 @@
         <v>13</v>
       </c>
       <c r="C21" s="1">
-        <v>0.1809350292162644</v>
+        <v>0.5452539943146544</v>
       </c>
       <c r="D21" s="1">
-        <v>0.8123476569107348</v>
+        <v>0.3730859340305037</v>
       </c>
       <c r="E21">
         <v>14</v>
@@ -1277,10 +1286,10 @@
         <v>14</v>
       </c>
       <c r="C22" s="1">
-        <v>0.1636447119069271</v>
+        <v>0.7656993893382078</v>
       </c>
       <c r="D22" s="1">
-        <v>0.8059151036038091</v>
+        <v>0.1988705560760465</v>
       </c>
       <c r="E22">
         <v>13</v>
@@ -1294,10 +1303,10 @@
         <v>15</v>
       </c>
       <c r="C23" s="1">
-        <v>0.1381611054857339</v>
+        <v>0.8346920127058352</v>
       </c>
       <c r="D23" s="1">
-        <v>0.7574638473677997</v>
+        <v>0.1406221465654954</v>
       </c>
       <c r="E23">
         <v>12</v>
@@ -1311,10 +1320,10 @@
         <v>16</v>
       </c>
       <c r="C24" s="1">
-        <v>0.2282825262821861</v>
+        <v>0.7274706849640297</v>
       </c>
       <c r="D24" s="1">
-        <v>0.8170294457232519</v>
+        <v>0.188223641739365</v>
       </c>
       <c r="E24">
         <v>11</v>
@@ -1328,10 +1337,10 @@
         <v>17</v>
       </c>
       <c r="C25" s="1">
-        <v>0.2276192464347997</v>
+        <v>0.9096400134282258</v>
       </c>
       <c r="D25" s="1">
-        <v>0.7904972105057587</v>
+        <v>0.10753769620323</v>
       </c>
       <c r="E25">
         <v>10</v>
@@ -1345,10 +1354,10 @@
         <v>18</v>
       </c>
       <c r="C26" s="1">
-        <v>0.3663844860194911</v>
+        <v>0.9261676110347306</v>
       </c>
       <c r="D26" s="1">
-        <v>0.6868570095767319</v>
+        <v>0.031986823289332</v>
       </c>
       <c r="E26">
         <v>9</v>
@@ -1362,10 +1371,10 @@
         <v>19</v>
       </c>
       <c r="C27" s="1">
-        <v>0.3652077072120486</v>
+        <v>0.9453144100552824</v>
       </c>
       <c r="D27" s="1">
-        <v>0.678462449211344</v>
+        <v>0</v>
       </c>
       <c r="E27">
         <v>8</v>
@@ -1379,10 +1388,10 @@
         <v>20</v>
       </c>
       <c r="C28" s="1">
-        <v>0.4065624587608148</v>
+        <v>1</v>
       </c>
       <c r="D28" s="1">
-        <v>0.7349813382823553</v>
+        <v>0</v>
       </c>
       <c r="E28">
         <v>7</v>
@@ -1396,10 +1405,10 @@
         <v>21</v>
       </c>
       <c r="C29" s="1">
-        <v>0.3750525719654789</v>
+        <v>0.9795071410359218</v>
       </c>
       <c r="D29" s="1">
-        <v>0.6364863328227983</v>
+        <v>0</v>
       </c>
       <c r="E29">
         <v>6</v>
@@ -1413,10 +1422,10 @@
         <v>22</v>
       </c>
       <c r="C30" s="1">
-        <v>0.402773541720006</v>
+        <v>1</v>
       </c>
       <c r="D30" s="1">
-        <v>0.7398683720896356</v>
+        <v>0.09827170168442574</v>
       </c>
       <c r="E30">
         <v>5</v>
@@ -1430,10 +1439,10 @@
         <v>23</v>
       </c>
       <c r="C31" s="1">
-        <v>0.4116730285605797</v>
+        <v>1</v>
       </c>
       <c r="D31" s="1">
-        <v>0.7322917929956112</v>
+        <v>0</v>
       </c>
       <c r="E31">
         <v>4</v>
@@ -1447,10 +1456,10 @@
         <v>24</v>
       </c>
       <c r="C32" s="1">
-        <v>0.2284720697855734</v>
+        <v>1</v>
       </c>
       <c r="D32" s="1">
-        <v>0.6812152183654794</v>
+        <v>0</v>
       </c>
       <c r="E32">
         <v>3</v>
@@ -1464,10 +1473,10 @@
         <v>25</v>
       </c>
       <c r="C33" s="1">
-        <v>0.4324044374920852</v>
+        <v>0.9757517052346958</v>
       </c>
       <c r="D33" s="1">
-        <v>0.6872980780634957</v>
+        <v>0.03600326541959095</v>
       </c>
       <c r="E33">
         <v>2</v>
@@ -1479,6 +1488,9 @@
       </c>
       <c r="B34">
         <v>26</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1</v>
       </c>
       <c r="E34">
         <v>1</v>

</xml_diff>

<commit_message>
28.10.21 more work for full intact ion mode: Functionality works until IntactSpectrumHandler (basically tested)
</commit_message>
<xml_diff>
--- a/Spectral_data/Occupancies_out.xlsx
+++ b/Spectral_data/Occupancies_out.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="12">
   <si>
-    <t>16/07/2021 09:26</t>
+    <t>28/10/2021 14:19</t>
   </si>
   <si>
     <t>fragmentation:</t>
@@ -31,7 +31,7 @@
     <t>Occupancies: /%</t>
   </si>
   <si>
-    <t>base'</t>
+    <t>building block'</t>
   </si>
   <si>
     <t>G</t>
@@ -240,6 +240,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
@@ -250,55 +253,55 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.1824670653632344</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.3713393219524556</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.4524467626064254</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.297255549154257</c:v>
+                  <c:v>0.04341778151384942</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.4311368899685053</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.435889064979885</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.5452539943146544</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.7656993893382078</c:v>
+                  <c:v>0.08832295677369027</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.8346920127058352</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.7274706849640297</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.9096400134282258</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.9261676110347306</c:v>
+                  <c:v>0.07915796045487891</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.9453144100552824</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>0.3851899325008479</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.9795071410359218</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>1</c:v>
@@ -310,7 +313,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.9757517052346958</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>1</c:v>
@@ -445,64 +448,64 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.04088863556810497</c:v>
+                  <c:v>0.9541370359300535</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.775330355050239</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.8701710938353409</c:v>
+                  <c:v>0.9233236455587249</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.6350668206904492</c:v>
+                  <c:v>0.7625383129883069</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.4409841597897683</c:v>
+                  <c:v>0.7983817169069879</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.5690547461769253</c:v>
+                  <c:v>0.8684256221000354</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.6599488907230143</c:v>
+                  <c:v>0.9551704335076069</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.4150167147834023</c:v>
+                  <c:v>0.8712357146846603</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.4733584948958165</c:v>
+                  <c:v>0.7919427833912946</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.3730859340305037</c:v>
+                  <c:v>0.7953734055766429</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.1988705560760465</c:v>
+                  <c:v>0.7637402168832881</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.1406221465654954</c:v>
+                  <c:v>0.7690488990429998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.188223641739365</c:v>
+                  <c:v>0.7271058842128088</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.10753769620323</c:v>
+                  <c:v>0.7110310758428157</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.031986823289332</c:v>
+                  <c:v>0.6640704502901278</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>0.750919542782607</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>0.3090154625760785</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.09827170168442574</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0</c:v>
@@ -511,7 +514,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.03600326541959095</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1027,7 +1030,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>0.3746581944490083</v>
+        <v>0.4824312578484021</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1035,7 +1038,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>0.6253418055509914</v>
+        <v>0.5175687421515976</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1067,6 +1070,9 @@
       <c r="B9">
         <v>1</v>
       </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
       <c r="D9" s="1">
         <v>1</v>
       </c>
@@ -1102,7 +1108,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="1">
-        <v>0.04088863556810497</v>
+        <v>0.9541370359300535</v>
       </c>
       <c r="E11">
         <v>24</v>
@@ -1119,7 +1125,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="1">
-        <v>0.775330355050239</v>
+        <v>1</v>
       </c>
       <c r="E12">
         <v>23</v>
@@ -1133,7 +1139,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="1">
-        <v>0.1824670653632344</v>
+        <v>0</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
@@ -1153,7 +1159,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="1">
-        <v>0.8701710938353409</v>
+        <v>0.9233236455587249</v>
       </c>
       <c r="E14">
         <v>21</v>
@@ -1167,10 +1173,10 @@
         <v>7</v>
       </c>
       <c r="C15" s="1">
-        <v>0.3713393219524556</v>
+        <v>0</v>
       </c>
       <c r="D15" s="1">
-        <v>0.6350668206904492</v>
+        <v>0.7625383129883069</v>
       </c>
       <c r="E15">
         <v>20</v>
@@ -1184,10 +1190,10 @@
         <v>8</v>
       </c>
       <c r="C16" s="1">
-        <v>0.4524467626064254</v>
+        <v>0</v>
       </c>
       <c r="D16" s="1">
-        <v>0.4409841597897683</v>
+        <v>0.7983817169069879</v>
       </c>
       <c r="E16">
         <v>19</v>
@@ -1201,10 +1207,10 @@
         <v>9</v>
       </c>
       <c r="C17" s="1">
-        <v>0.297255549154257</v>
+        <v>0.04341778151384942</v>
       </c>
       <c r="D17" s="1">
-        <v>0.5690547461769253</v>
+        <v>0.8684256221000354</v>
       </c>
       <c r="E17">
         <v>18</v>
@@ -1218,10 +1224,10 @@
         <v>10</v>
       </c>
       <c r="C18" s="1">
-        <v>0.4311368899685053</v>
+        <v>0</v>
       </c>
       <c r="D18" s="1">
-        <v>0.6599488907230143</v>
+        <v>0.9551704335076069</v>
       </c>
       <c r="E18">
         <v>17</v>
@@ -1238,7 +1244,7 @@
         <v>0</v>
       </c>
       <c r="D19" s="1">
-        <v>0.4150167147834023</v>
+        <v>0.8712357146846603</v>
       </c>
       <c r="E19">
         <v>16</v>
@@ -1252,10 +1258,10 @@
         <v>12</v>
       </c>
       <c r="C20" s="1">
-        <v>0.435889064979885</v>
+        <v>0</v>
       </c>
       <c r="D20" s="1">
-        <v>0.4733584948958165</v>
+        <v>0.7919427833912946</v>
       </c>
       <c r="E20">
         <v>15</v>
@@ -1269,10 +1275,10 @@
         <v>13</v>
       </c>
       <c r="C21" s="1">
-        <v>0.5452539943146544</v>
+        <v>0</v>
       </c>
       <c r="D21" s="1">
-        <v>0.3730859340305037</v>
+        <v>0.7953734055766429</v>
       </c>
       <c r="E21">
         <v>14</v>
@@ -1286,10 +1292,10 @@
         <v>14</v>
       </c>
       <c r="C22" s="1">
-        <v>0.7656993893382078</v>
+        <v>0.08832295677369027</v>
       </c>
       <c r="D22" s="1">
-        <v>0.1988705560760465</v>
+        <v>0.7637402168832881</v>
       </c>
       <c r="E22">
         <v>13</v>
@@ -1303,10 +1309,10 @@
         <v>15</v>
       </c>
       <c r="C23" s="1">
-        <v>0.8346920127058352</v>
+        <v>0</v>
       </c>
       <c r="D23" s="1">
-        <v>0.1406221465654954</v>
+        <v>0.7690488990429998</v>
       </c>
       <c r="E23">
         <v>12</v>
@@ -1320,10 +1326,10 @@
         <v>16</v>
       </c>
       <c r="C24" s="1">
-        <v>0.7274706849640297</v>
+        <v>0</v>
       </c>
       <c r="D24" s="1">
-        <v>0.188223641739365</v>
+        <v>0.7271058842128088</v>
       </c>
       <c r="E24">
         <v>11</v>
@@ -1337,10 +1343,10 @@
         <v>17</v>
       </c>
       <c r="C25" s="1">
-        <v>0.9096400134282258</v>
+        <v>0</v>
       </c>
       <c r="D25" s="1">
-        <v>0.10753769620323</v>
+        <v>0.7110310758428157</v>
       </c>
       <c r="E25">
         <v>10</v>
@@ -1354,10 +1360,10 @@
         <v>18</v>
       </c>
       <c r="C26" s="1">
-        <v>0.9261676110347306</v>
+        <v>0.07915796045487891</v>
       </c>
       <c r="D26" s="1">
-        <v>0.031986823289332</v>
+        <v>0.6640704502901278</v>
       </c>
       <c r="E26">
         <v>9</v>
@@ -1371,10 +1377,10 @@
         <v>19</v>
       </c>
       <c r="C27" s="1">
-        <v>0.9453144100552824</v>
+        <v>0</v>
       </c>
       <c r="D27" s="1">
-        <v>0</v>
+        <v>0.750919542782607</v>
       </c>
       <c r="E27">
         <v>8</v>
@@ -1388,10 +1394,10 @@
         <v>20</v>
       </c>
       <c r="C28" s="1">
-        <v>1</v>
+        <v>0.3851899325008479</v>
       </c>
       <c r="D28" s="1">
-        <v>0</v>
+        <v>0.3090154625760785</v>
       </c>
       <c r="E28">
         <v>7</v>
@@ -1405,7 +1411,7 @@
         <v>21</v>
       </c>
       <c r="C29" s="1">
-        <v>0.9795071410359218</v>
+        <v>1</v>
       </c>
       <c r="D29" s="1">
         <v>0</v>
@@ -1425,7 +1431,7 @@
         <v>1</v>
       </c>
       <c r="D30" s="1">
-        <v>0.09827170168442574</v>
+        <v>0</v>
       </c>
       <c r="E30">
         <v>5</v>
@@ -1473,10 +1479,10 @@
         <v>25</v>
       </c>
       <c r="C33" s="1">
-        <v>0.9757517052346958</v>
+        <v>1</v>
       </c>
       <c r="D33" s="1">
-        <v>0.03600326541959095</v>
+        <v>0</v>
       </c>
       <c r="E33">
         <v>2</v>

</xml_diff>

<commit_message>
24.11.21 Calculation of isotope patterns can be accelerated (FFT) reorganisation of parameter dialog
</commit_message>
<xml_diff>
--- a/Spectral_data/Occupancies_out.xlsx
+++ b/Spectral_data/Occupancies_out.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
   <si>
-    <t>28/10/2021 14:19</t>
+    <t>23/11/2021 15:25</t>
   </si>
   <si>
     <t>fragmentation:</t>
@@ -37,13 +37,13 @@
     <t>G</t>
   </si>
   <si>
+    <t>A</t>
+  </si>
+  <si>
     <t>C</t>
   </si>
   <si>
     <t>U</t>
-  </si>
-  <si>
-    <t>A</t>
   </si>
   <si>
     <t>#5'/N-term.</t>
@@ -146,10 +146,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>analysis!$B$9:$B$35</c:f>
+              <c:f>analysis!$B$9:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -194,52 +194,16 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>analysis!$C$9:$C$35</c:f>
+              <c:f>analysis!$C$9:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -259,64 +223,28 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.04341778151384942</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.08832295677369027</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.07915796045487891</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.3851899325008479</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1</c:v>
+                  <c:v>0.9637717070821593</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -347,10 +275,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>analysis!$B$9:$B$35</c:f>
+              <c:f>analysis!$B$9:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -395,52 +323,16 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>analysis!$D$9:$D$35</c:f>
+              <c:f>analysis!$D$9:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -448,7 +340,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.9541370359300535</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
@@ -457,63 +349,27 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.9233236455587249</c:v>
+                  <c:v>0.9369518304598258</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.7625383129883069</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.7983817169069879</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.8684256221000354</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.9551704335076069</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.8712357146846603</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.7919427833912946</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.7953734055766429</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.7637402168832881</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.7690488990429998</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.7271058842128088</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.7110310758428157</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.6640704502901278</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.750919542782607</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.3090154625760785</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="24">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -607,7 +463,7 @@
         </c:txPr>
         <c:crossAx val="50010001"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="50010004"/>
@@ -701,8 +557,8 @@
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
@@ -1011,7 +867,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1030,7 +886,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>0.4824312578484021</v>
+        <v>0.5452711978133886</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1038,7 +894,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>0.5175687421515976</v>
+        <v>0.4547288021866113</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1077,12 +933,12 @@
         <v>1</v>
       </c>
       <c r="E9">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -1094,7 +950,7 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1108,15 +964,15 @@
         <v>0</v>
       </c>
       <c r="D11" s="1">
-        <v>0.9541370359300535</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B12">
         <v>4</v>
@@ -1128,7 +984,7 @@
         <v>1</v>
       </c>
       <c r="E12">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1145,12 +1001,12 @@
         <v>1</v>
       </c>
       <c r="E13">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14">
         <v>6</v>
@@ -1159,10 +1015,10 @@
         <v>0</v>
       </c>
       <c r="D14" s="1">
-        <v>0.9233236455587249</v>
+        <v>0.9369518304598258</v>
       </c>
       <c r="E14">
-        <v>21</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1173,47 +1029,47 @@
         <v>7</v>
       </c>
       <c r="C15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="1">
-        <v>0.7625383129883069</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16">
         <v>8</v>
       </c>
       <c r="C16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="1">
-        <v>0.7983817169069879</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B17">
         <v>9</v>
       </c>
       <c r="C17" s="1">
-        <v>0.04341778151384942</v>
+        <v>1</v>
       </c>
       <c r="D17" s="1">
-        <v>0.8684256221000354</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1224,64 +1080,64 @@
         <v>10</v>
       </c>
       <c r="C18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="1">
-        <v>0.9551704335076069</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B19">
         <v>11</v>
       </c>
       <c r="C19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="1">
-        <v>0.8712357146846603</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B20">
         <v>12</v>
       </c>
       <c r="C20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="1">
-        <v>0.7919427833912946</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B21">
         <v>13</v>
       </c>
       <c r="C21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="1">
-        <v>0.7953734055766429</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1292,222 +1148,18 @@
         <v>14</v>
       </c>
       <c r="C22" s="1">
-        <v>0.08832295677369027</v>
-      </c>
-      <c r="D22" s="1">
-        <v>0.7637402168832881</v>
+        <v>0.9637717070821593</v>
       </c>
       <c r="E22">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B23">
         <v>15</v>
-      </c>
-      <c r="C23" s="1">
-        <v>0</v>
-      </c>
-      <c r="D23" s="1">
-        <v>0.7690488990429998</v>
-      </c>
-      <c r="E23">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24">
-        <v>16</v>
-      </c>
-      <c r="C24" s="1">
-        <v>0</v>
-      </c>
-      <c r="D24" s="1">
-        <v>0.7271058842128088</v>
-      </c>
-      <c r="E24">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25">
-        <v>17</v>
-      </c>
-      <c r="C25" s="1">
-        <v>0</v>
-      </c>
-      <c r="D25" s="1">
-        <v>0.7110310758428157</v>
-      </c>
-      <c r="E25">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26">
-        <v>18</v>
-      </c>
-      <c r="C26" s="1">
-        <v>0.07915796045487891</v>
-      </c>
-      <c r="D26" s="1">
-        <v>0.6640704502901278</v>
-      </c>
-      <c r="E26">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27">
-        <v>19</v>
-      </c>
-      <c r="C27" s="1">
-        <v>0</v>
-      </c>
-      <c r="D27" s="1">
-        <v>0.750919542782607</v>
-      </c>
-      <c r="E27">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28">
-        <v>20</v>
-      </c>
-      <c r="C28" s="1">
-        <v>0.3851899325008479</v>
-      </c>
-      <c r="D28" s="1">
-        <v>0.3090154625760785</v>
-      </c>
-      <c r="E28">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" t="s">
-        <v>8</v>
-      </c>
-      <c r="B29">
-        <v>21</v>
-      </c>
-      <c r="C29" s="1">
-        <v>1</v>
-      </c>
-      <c r="D29" s="1">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30">
-        <v>22</v>
-      </c>
-      <c r="C30" s="1">
-        <v>1</v>
-      </c>
-      <c r="D30" s="1">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31">
-        <v>23</v>
-      </c>
-      <c r="C31" s="1">
-        <v>1</v>
-      </c>
-      <c r="D31" s="1">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" t="s">
-        <v>9</v>
-      </c>
-      <c r="B32">
-        <v>24</v>
-      </c>
-      <c r="C32" s="1">
-        <v>1</v>
-      </c>
-      <c r="D32" s="1">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33">
-        <v>25</v>
-      </c>
-      <c r="C33" s="1">
-        <v>1</v>
-      </c>
-      <c r="D33" s="1">
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" t="s">
-        <v>8</v>
-      </c>
-      <c r="B34">
-        <v>26</v>
-      </c>
-      <c r="C34" s="1">
-        <v>1</v>
-      </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
03.12.21 fixed bugs: * calc.abs.occupancy: unmodified value was sum of modified+unmodified instead of just unmodified
</commit_message>
<xml_diff>
--- a/Spectral_data/Occupancies_out.xlsx
+++ b/Spectral_data/Occupancies_out.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
   <si>
-    <t>23/11/2021 15:25</t>
+    <t>02/12/2021 15:56</t>
   </si>
   <si>
     <t>fragmentation:</t>
@@ -34,16 +34,16 @@
     <t>building block'</t>
   </si>
   <si>
+    <t>C</t>
+  </si>
+  <si>
     <t>G</t>
   </si>
   <si>
-    <t>A</t>
+    <t>U</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>U</t>
+    <t>A</t>
   </si>
   <si>
     <t>#5'/N-term.</t>
@@ -146,10 +146,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>analysis!$B$9:$B$23</c:f>
+              <c:f>analysis!$B$9:$B$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -194,57 +194,90 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>analysis!$C$9:$C$23</c:f>
+              <c:f>analysis!$C$9:$C$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
+                <c:ptCount val="22"/>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.4156929710392711</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.1184307673440473</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.2239676350944688</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>0.1221181154312463</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.06739069687733443</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.2398960822704143</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.3892407751320323</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.4922115374019348</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.4037097862374647</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="14">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="15">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="16">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="17">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="19">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="20">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.9637717070821593</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -275,10 +308,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>analysis!$B$9:$B$23</c:f>
+              <c:f>analysis!$B$9:$B$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -323,53 +356,92 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>analysis!$D$9:$D$23</c:f>
+              <c:f>analysis!$D$9:$D$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0.8903428667669734</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0.9100201352285989</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.9369518304598258</c:v>
+                  <c:v>0.7569672053455951</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>0.7099395662749711</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7819043364758039</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.7641921805006157</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.7380100504719854</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5664733395893607</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.4204433502250054</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.1683161361207938</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="14">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="15">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="16">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="17">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="18">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="19">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -557,8 +629,8 @@
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
@@ -867,7 +939,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -886,7 +958,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>0.5452711978133886</v>
+        <v>0.5073022904471499</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -894,7 +966,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>0.4547288021866113</v>
+        <v>0.49269770955285</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -926,14 +998,11 @@
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9" s="1">
-        <v>0</v>
-      </c>
       <c r="D9" s="1">
         <v>1</v>
       </c>
       <c r="E9">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -950,24 +1019,21 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B11">
         <v>3</v>
       </c>
       <c r="C11" s="1">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1</v>
+        <v>0.4156929710392711</v>
       </c>
       <c r="E11">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -981,61 +1047,61 @@
         <v>0</v>
       </c>
       <c r="D12" s="1">
-        <v>1</v>
+        <v>0.8903428667669734</v>
       </c>
       <c r="E12">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B13">
         <v>5</v>
       </c>
       <c r="C13" s="1">
-        <v>0</v>
+        <v>0.1184307673440473</v>
       </c>
       <c r="D13" s="1">
-        <v>1</v>
+        <v>0.9100201352285989</v>
       </c>
       <c r="E13">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B14">
         <v>6</v>
       </c>
       <c r="C14" s="1">
-        <v>0</v>
+        <v>0.2239676350944688</v>
       </c>
       <c r="D14" s="1">
-        <v>0.9369518304598258</v>
+        <v>0.7569672053455951</v>
       </c>
       <c r="E14">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B15">
         <v>7</v>
       </c>
       <c r="C15" s="1">
-        <v>1</v>
+        <v>0.1221181154312463</v>
       </c>
       <c r="D15" s="1">
-        <v>0</v>
+        <v>0.7099395662749711</v>
       </c>
       <c r="E15">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1046,98 +1112,95 @@
         <v>8</v>
       </c>
       <c r="C16" s="1">
-        <v>1</v>
+        <v>0.06739069687733443</v>
       </c>
       <c r="D16" s="1">
-        <v>0</v>
+        <v>0.7819043364758039</v>
       </c>
       <c r="E16">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B17">
         <v>9</v>
       </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
       <c r="D17" s="1">
-        <v>0</v>
+        <v>0.7641921805006157</v>
       </c>
       <c r="E17">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B18">
         <v>10</v>
       </c>
       <c r="C18" s="1">
-        <v>1</v>
+        <v>0.2398960822704143</v>
       </c>
       <c r="D18" s="1">
-        <v>0</v>
+        <v>0.7380100504719854</v>
       </c>
       <c r="E18">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19">
         <v>11</v>
       </c>
       <c r="C19" s="1">
-        <v>1</v>
+        <v>0.3892407751320323</v>
       </c>
       <c r="D19" s="1">
-        <v>0</v>
+        <v>0.5664733395893607</v>
       </c>
       <c r="E19">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B20">
         <v>12</v>
       </c>
       <c r="C20" s="1">
-        <v>1</v>
+        <v>0.4922115374019348</v>
       </c>
       <c r="D20" s="1">
-        <v>0</v>
+        <v>0.4204433502250054</v>
       </c>
       <c r="E20">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21">
         <v>13</v>
       </c>
       <c r="C21" s="1">
-        <v>1</v>
+        <v>0.4037097862374647</v>
       </c>
       <c r="D21" s="1">
-        <v>0</v>
+        <v>0.1683161361207938</v>
       </c>
       <c r="E21">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1148,10 +1211,13 @@
         <v>14</v>
       </c>
       <c r="C22" s="1">
-        <v>0.9637717070821593</v>
+        <v>1</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1160,6 +1226,119 @@
       </c>
       <c r="B23">
         <v>15</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24">
+        <v>16</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25">
+        <v>17</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26">
+        <v>18</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27">
+        <v>19</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28">
+        <v>20</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29">
+        <v>21</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
14.12. new: * Adding new ions that were already included (=overwriting) works * default json configuration files are created if the corresponding files do not exist * protocol text more informative for adding/changing ions bugs fixed: * in intact search: export dialog did not work * in Info.py: peak values not properly displayed when changing/adding ions
</commit_message>
<xml_diff>
--- a/Spectral_data/Occupancies_out.xlsx
+++ b/Spectral_data/Occupancies_out.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
   <si>
-    <t>02/12/2021 15:56</t>
+    <t>13/12/2021 11:54</t>
   </si>
   <si>
     <t>fragmentation:</t>
@@ -31,19 +31,19 @@
     <t>Occupancies: /%</t>
   </si>
   <si>
-    <t>building block'</t>
-  </si>
-  <si>
-    <t>C</t>
+    <t>building block</t>
   </si>
   <si>
     <t>G</t>
   </si>
   <si>
+    <t>A</t>
+  </si>
+  <si>
     <t>U</t>
   </si>
   <si>
-    <t>A</t>
+    <t>C</t>
   </si>
   <si>
     <t>#5'/N-term.</t>
@@ -146,10 +146,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>analysis!$B$9:$B$30</c:f>
+              <c:f>analysis!$B$9:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -194,89 +194,53 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>analysis!$C$9:$C$30</c:f>
+              <c:f>analysis!$C$9:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.4156929710392711</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.1184307673440473</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.2239676350944688</c:v>
+                  <c:v>0.139092390478553</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.1221181154312463</c:v>
+                  <c:v>0.8849763136359212</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.06739069687733443</c:v>
+                  <c:v>0.9454031632565497</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.2398960822704143</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.3892407751320323</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.4922115374019348</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.4037097862374647</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="20">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -308,10 +272,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>analysis!$B$9:$B$30</c:f>
+              <c:f>analysis!$B$9:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -356,92 +320,53 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>analysis!$D$9:$D$30</c:f>
+              <c:f>analysis!$D$9:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.8903428667669734</c:v>
+                  <c:v>0.827888116976033</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.9100201352285989</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.7569672053455951</c:v>
+                  <c:v>0.8003813815706204</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.7099395662749711</c:v>
+                  <c:v>0.153840896990948</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.7819043364758039</c:v>
+                  <c:v>0.04684674871205083</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.7641921805006157</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.7380100504719854</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.5664733395893607</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.4204433502250054</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.1683161361207938</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -629,8 +554,8 @@
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
@@ -939,7 +864,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -958,7 +883,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>0.5073022904471499</v>
+        <v>0.4987773732222749</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -966,7 +891,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>0.49269770955285</v>
+        <v>0.5012226267777251</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1002,7 +927,7 @@
         <v>1</v>
       </c>
       <c r="E9">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1019,21 +944,24 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11">
         <v>3</v>
       </c>
       <c r="C11" s="1">
-        <v>0.4156929710392711</v>
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1047,92 +975,95 @@
         <v>0</v>
       </c>
       <c r="D12" s="1">
-        <v>0.8903428667669734</v>
+        <v>0.827888116976033</v>
       </c>
       <c r="E12">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B13">
         <v>5</v>
       </c>
       <c r="C13" s="1">
-        <v>0.1184307673440473</v>
+        <v>0</v>
       </c>
       <c r="D13" s="1">
-        <v>0.9100201352285989</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B14">
         <v>6</v>
       </c>
       <c r="C14" s="1">
-        <v>0.2239676350944688</v>
+        <v>0.139092390478553</v>
       </c>
       <c r="D14" s="1">
-        <v>0.7569672053455951</v>
+        <v>0.8003813815706204</v>
       </c>
       <c r="E14">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B15">
         <v>7</v>
       </c>
       <c r="C15" s="1">
-        <v>0.1221181154312463</v>
+        <v>0.8849763136359212</v>
       </c>
       <c r="D15" s="1">
-        <v>0.7099395662749711</v>
+        <v>0.153840896990948</v>
       </c>
       <c r="E15">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B16">
         <v>8</v>
       </c>
       <c r="C16" s="1">
-        <v>0.06739069687733443</v>
+        <v>0.9454031632565497</v>
       </c>
       <c r="D16" s="1">
-        <v>0.7819043364758039</v>
+        <v>0.04684674871205083</v>
       </c>
       <c r="E16">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B17">
         <v>9</v>
       </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
       <c r="D17" s="1">
-        <v>0.7641921805006157</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1143,47 +1074,47 @@
         <v>10</v>
       </c>
       <c r="C18" s="1">
-        <v>0.2398960822704143</v>
+        <v>1</v>
       </c>
       <c r="D18" s="1">
-        <v>0.7380100504719854</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B19">
         <v>11</v>
       </c>
       <c r="C19" s="1">
-        <v>0.3892407751320323</v>
+        <v>1</v>
       </c>
       <c r="D19" s="1">
-        <v>0.5664733395893607</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B20">
         <v>12</v>
       </c>
       <c r="C20" s="1">
-        <v>0.4922115374019348</v>
+        <v>1</v>
       </c>
       <c r="D20" s="1">
-        <v>0.4204433502250054</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1194,18 +1125,18 @@
         <v>13</v>
       </c>
       <c r="C21" s="1">
-        <v>0.4037097862374647</v>
+        <v>1</v>
       </c>
       <c r="D21" s="1">
-        <v>0.1683161361207938</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B22">
         <v>14</v>
@@ -1213,11 +1144,8 @@
       <c r="C22" s="1">
         <v>1</v>
       </c>
-      <c r="D22" s="1">
-        <v>0</v>
-      </c>
       <c r="E22">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1226,119 +1154,6 @@
       </c>
       <c r="B23">
         <v>15</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1</v>
-      </c>
-      <c r="D23" s="1">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24">
-        <v>16</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1</v>
-      </c>
-      <c r="D24" s="1">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25">
-        <v>17</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1</v>
-      </c>
-      <c r="D25" s="1">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26">
-        <v>18</v>
-      </c>
-      <c r="C26" s="1">
-        <v>1</v>
-      </c>
-      <c r="D26" s="1">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27">
-        <v>19</v>
-      </c>
-      <c r="D27" s="1">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" t="s">
-        <v>8</v>
-      </c>
-      <c r="B28">
-        <v>20</v>
-      </c>
-      <c r="C28" s="1">
-        <v>1</v>
-      </c>
-      <c r="D28" s="1">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29">
-        <v>21</v>
-      </c>
-      <c r="C29" s="1">
-        <v>1</v>
-      </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
15.07.22: fixed bug in calculating site-specific abundances for each fragment
</commit_message>
<xml_diff>
--- a/Spectral_data/Occupancies_out.xlsx
+++ b/Spectral_data/Occupancies_out.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="12">
   <si>
-    <t>13/12/2021 11:54</t>
+    <t>08/07/2022 12:23</t>
   </si>
   <si>
     <t>fragmentation:</t>
@@ -28,7 +28,7 @@
     <t>y</t>
   </si>
   <si>
-    <t>Occupancies: /%</t>
+    <t>Occupancies: +CMC /%</t>
   </si>
   <si>
     <t>building block</t>
@@ -37,13 +37,13 @@
     <t>G</t>
   </si>
   <si>
-    <t>A</t>
+    <t>C</t>
   </si>
   <si>
     <t>U</t>
   </si>
   <si>
-    <t>C</t>
+    <t>A</t>
   </si>
   <si>
     <t>#5'/N-term.</t>
@@ -116,7 +116,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Occupancies</a:t>
+              <a:t>Occupancies: +CMC</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -146,10 +146,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>analysis!$B$9:$B$23</c:f>
+              <c:f>analysis!$B$9:$B$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -194,16 +194,55 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>analysis!$C$9:$C$23</c:f>
+              <c:f>analysis!$C$9:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
@@ -211,36 +250,72 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.03980944833814252</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.139092390478553</c:v>
+                  <c:v>0.03726120037346731</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.8849763136359212</c:v>
+                  <c:v>0.5479614367576472</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.9454031632565497</c:v>
+                  <c:v>0.5887740674227893</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>0.5932694395284328</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.6252010848421716</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.3095449201614789</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.642857240785801</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.7626317984591211</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.8694990353270214</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.9265356110671655</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.8852062602754215</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.9089101300792869</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.9436890539038481</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.9402403422226534</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="20">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="21">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="22">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="23">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="24">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -272,10 +347,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>analysis!$B$9:$B$23</c:f>
+              <c:f>analysis!$B$9:$B$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -320,16 +395,52 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>analysis!$D$9:$D$23</c:f>
+              <c:f>analysis!$D$9:$D$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -340,33 +451,69 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.827888116976033</c:v>
+                  <c:v>0.8217830605474922</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>0.8791288789142748</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7979057149243461</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.8003813815706204</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.153840896990948</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.04684674871205083</c:v>
+                  <c:v>0.3577475090367369</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>0.2924351879928614</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.3279777598250497</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.3139148342463861</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.2232182792244859</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.1838262212045511</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.1353400482199481</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.07733731758926685</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.05700219732802908</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.08244393717602493</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.05018492158030112</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.04662869757102946</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="20">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="21">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="22">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -439,7 +586,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1300" baseline="0"/>
-                  <a:t>5'-O /%</a:t>
+                  <a:t>O (5'/N-term.) /%</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -481,7 +628,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1300" baseline="0"/>
-                  <a:t>3'-O /%</a:t>
+                  <a:t>O (3'/C-term.) /%</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -554,8 +701,8 @@
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
@@ -864,7 +1011,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -883,7 +1030,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>0.4987773732222749</v>
+        <v>0.4532387272333573</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -891,7 +1038,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>0.5012226267777251</v>
+        <v>0.5467612727666429</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -923,16 +1070,19 @@
       <c r="B9">
         <v>1</v>
       </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
       <c r="D9" s="1">
         <v>1</v>
       </c>
       <c r="E9">
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -944,7 +1094,7 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -961,24 +1111,24 @@
         <v>1</v>
       </c>
       <c r="E11">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B12">
         <v>4</v>
       </c>
       <c r="C12" s="1">
-        <v>0</v>
+        <v>0.03980944833814252</v>
       </c>
       <c r="D12" s="1">
-        <v>0.827888116976033</v>
+        <v>0.8217830605474922</v>
       </c>
       <c r="E12">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -992,27 +1142,27 @@
         <v>0</v>
       </c>
       <c r="D13" s="1">
-        <v>1</v>
+        <v>0.8791288789142748</v>
       </c>
       <c r="E13">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14">
         <v>6</v>
       </c>
       <c r="C14" s="1">
-        <v>0.139092390478553</v>
+        <v>0.03726120037346731</v>
       </c>
       <c r="D14" s="1">
-        <v>0.8003813815706204</v>
+        <v>0.7979057149243461</v>
       </c>
       <c r="E14">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1023,30 +1173,30 @@
         <v>7</v>
       </c>
       <c r="C15" s="1">
-        <v>0.8849763136359212</v>
+        <v>0.5479614367576472</v>
       </c>
       <c r="D15" s="1">
-        <v>0.153840896990948</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16">
         <v>8</v>
       </c>
       <c r="C16" s="1">
-        <v>0.9454031632565497</v>
+        <v>0.5887740674227893</v>
       </c>
       <c r="D16" s="1">
-        <v>0.04684674871205083</v>
+        <v>0.3577475090367369</v>
       </c>
       <c r="E16">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1057,64 +1207,64 @@
         <v>9</v>
       </c>
       <c r="C17" s="1">
-        <v>1</v>
+        <v>0.5932694395284328</v>
       </c>
       <c r="D17" s="1">
-        <v>0</v>
+        <v>0.2924351879928614</v>
       </c>
       <c r="E17">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18">
         <v>10</v>
       </c>
       <c r="C18" s="1">
-        <v>1</v>
+        <v>0.6252010848421716</v>
       </c>
       <c r="D18" s="1">
-        <v>0</v>
+        <v>0.3279777598250497</v>
       </c>
       <c r="E18">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B19">
         <v>11</v>
       </c>
       <c r="C19" s="1">
-        <v>1</v>
+        <v>0.3095449201614789</v>
       </c>
       <c r="D19" s="1">
-        <v>0</v>
+        <v>0.3139148342463861</v>
       </c>
       <c r="E19">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20">
         <v>12</v>
       </c>
       <c r="C20" s="1">
-        <v>1</v>
+        <v>0.642857240785801</v>
       </c>
       <c r="D20" s="1">
-        <v>0</v>
+        <v>0.2232182792244859</v>
       </c>
       <c r="E20">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1125,35 +1275,239 @@
         <v>13</v>
       </c>
       <c r="C21" s="1">
-        <v>1</v>
+        <v>0.7626317984591211</v>
       </c>
       <c r="D21" s="1">
-        <v>0</v>
+        <v>0.1838262212045511</v>
       </c>
       <c r="E21">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22">
         <v>14</v>
       </c>
       <c r="C22" s="1">
-        <v>1</v>
+        <v>0.8694990353270214</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.1353400482199481</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B23">
         <v>15</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.9265356110671655</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.07733731758926685</v>
+      </c>
+      <c r="E23">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24">
+        <v>16</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.8852062602754215</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.05700219732802908</v>
+      </c>
+      <c r="E24">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>17</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.9089101300792869</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.08244393717602493</v>
+      </c>
+      <c r="E25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26">
+        <v>18</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0.9436890539038481</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.05018492158030112</v>
+      </c>
+      <c r="E26">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27">
+        <v>19</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.9402403422226534</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0.04662869757102946</v>
+      </c>
+      <c r="E27">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28">
+        <v>20</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29">
+        <v>21</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30">
+        <v>22</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31">
+        <v>23</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32">
+        <v>24</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33">
+        <v>25</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34">
+        <v>26</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>